<commit_message>
- e coli protein toolkit and open reporters all changed to local sequence file
</commit_message>
<xml_diff>
--- a/E coli Protein Expression Toolkit/E coli Protein Expression Toolkit.xlsx
+++ b/E coli Protein Expression Toolkit/E coli Protein Expression Toolkit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/E coli Protein Expression Toolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2089390-776A-E041-AD49-6403BDF392FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41098154-5D27-DF4C-9682-C9D886F27B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19700" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34260" yWindow="3460" windowWidth="30960" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23002,309 +23002,9 @@
     <t>EF_TZ</t>
   </si>
   <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003373.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003375.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003376.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003378.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003379.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003380.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003384.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003385.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003386.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003387.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003388.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003389.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003390.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003391.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003392.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003393.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003395.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003396.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003397.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003398.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003399.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003400.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003401.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003402.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003403.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003404.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003405.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003406.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003407.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003408.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003409.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003410.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003411.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003412.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003413.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003414.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003415.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003416.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003417.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003418.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003419.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003420.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003421.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003422.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003423.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003424.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003425.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003426.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003427.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003428.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003429.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003430.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003431.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003432.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003433.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003434.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003436.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003437.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003438.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003439.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003440.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003441.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003442.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003443.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003444.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003445.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003446.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003447.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003448.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003449.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003450.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003451.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003452.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003453.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003454.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003455.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003457.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003459.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003460.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003461.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003462.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003463.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003464.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003465.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003466.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003467.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003468.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003469.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003470.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003471.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003472.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003473.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003474.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003475.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003476.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003477.gb</t>
-  </si>
-  <si>
     <t>Open Bioeconomy Lab</t>
   </si>
   <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003332.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003333.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003356.gb</t>
-  </si>
-  <si>
-    <t>https://freegenes.github.io/genbank/BBF10K_003366.gb</t>
-  </si>
-  <si>
     <t>Taken directly from E. coli Protein Expression Toolkit at FreeGenes</t>
   </si>
   <si>
@@ -23312,6 +23012,306 @@
   </si>
   <si>
     <t>E. coli Protein Expression Toolkit</t>
+  </si>
+  <si>
+    <t>BBF10K_003332.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003333.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003356.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003366.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003373.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003375.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003376.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003378.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003379.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003380.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003384.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003385.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003386.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003387.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003388.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003389.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003390.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003391.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003392.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003393.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003395.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003396.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003397.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003398.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003399.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003400.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003401.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003402.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003403.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003404.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003405.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003406.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003407.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003408.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003409.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003410.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003411.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003412.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003413.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003414.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003415.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003416.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003417.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003418.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003419.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003420.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003421.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003422.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003423.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003424.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003425.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003426.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003427.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003428.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003429.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003430.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003431.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003432.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003433.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003434.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003436.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003437.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003438.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003439.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003440.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003441.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003442.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003443.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003444.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003445.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003446.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003447.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003448.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003449.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003450.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003451.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003452.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003453.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003454.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003455.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003457.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003459.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003460.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003461.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003462.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003463.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003464.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003465.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003466.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003467.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003468.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003469.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003470.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003471.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003472.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003473.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003474.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003475.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003476.gb</t>
+  </si>
+  <si>
+    <t>BBF10K_003477.gb</t>
   </si>
 </sst>
 </file>
@@ -23670,7 +23670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23728,14 +23728,12 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -24187,8 +24185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24212,7 +24210,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7735</v>
+        <v>7635</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
@@ -24226,7 +24224,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7728</v>
+        <v>7632</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -24262,14 +24260,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="51" t="s">
-        <v>7734</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53"/>
+      <c r="A5" s="52" t="s">
+        <v>7634</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24521,7 +24519,7 @@
         <v>47</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>7445</v>
@@ -24530,10 +24528,10 @@
         <v>7532</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G15" s="56" t="s">
-        <v>7729</v>
+        <v>7521</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7636</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18" t="s">
@@ -24559,7 +24557,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>7445</v>
@@ -24568,10 +24566,10 @@
         <v>7533</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G16" s="56" t="s">
-        <v>7730</v>
+        <v>7521</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7637</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18" t="s">
@@ -24597,7 +24595,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>7445</v>
@@ -24606,10 +24604,10 @@
         <v>7534</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>7731</v>
+        <v>7521</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7638</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18" t="s">
@@ -24635,7 +24633,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>7445</v>
@@ -24644,10 +24642,10 @@
         <v>7535</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G18" s="56" t="s">
-        <v>7732</v>
+        <v>7521</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7639</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18" t="s">
@@ -24666,26 +24664,26 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="51" t="s">
         <v>7536</v>
       </c>
       <c r="B19" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="51" t="s">
         <v>7536</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G19" s="55" t="s">
-        <v>7632</v>
+        <v>7521</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7640</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
@@ -24704,26 +24702,26 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="51" t="s">
         <v>7537</v>
       </c>
       <c r="B20" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="51" t="s">
         <v>7537</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G20" s="55" t="s">
-        <v>7633</v>
+        <v>7521</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7641</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
@@ -24742,26 +24740,26 @@
       <c r="M20" s="22"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="51" t="s">
         <v>7538</v>
       </c>
       <c r="B21" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="51" t="s">
         <v>7538</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G21" s="55" t="s">
-        <v>7634</v>
+        <v>7521</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7642</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18" t="s">
@@ -24780,26 +24778,26 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="51" t="s">
         <v>7539</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="51" t="s">
         <v>7539</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G22" s="55" t="s">
-        <v>7635</v>
+        <v>7521</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7643</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
@@ -24818,26 +24816,26 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="51" t="s">
         <v>7540</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="51" t="s">
         <v>7540</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G23" s="55" t="s">
-        <v>7636</v>
+        <v>7521</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7644</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18" t="s">
@@ -24856,26 +24854,26 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="51" t="s">
         <v>7541</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="51" t="s">
         <v>7541</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G24" s="55" t="s">
-        <v>7637</v>
+        <v>7521</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7645</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18" t="s">
@@ -24894,26 +24892,26 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="51" t="s">
         <v>7542</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="51" t="s">
         <v>7542</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G25" s="55" t="s">
-        <v>7638</v>
+        <v>7521</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7646</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
@@ -24932,26 +24930,26 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="51" t="s">
         <v>7543</v>
       </c>
       <c r="B26" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="51" t="s">
         <v>7543</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G26" s="55" t="s">
-        <v>7639</v>
+        <v>7521</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7647</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="18" t="s">
@@ -24970,26 +24968,26 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="51" t="s">
         <v>7544</v>
       </c>
       <c r="B27" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="51" t="s">
         <v>7544</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G27" s="55" t="s">
-        <v>7640</v>
+        <v>7521</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7648</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18" t="s">
@@ -25008,26 +25006,26 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="51" t="s">
         <v>7545</v>
       </c>
       <c r="B28" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="51" t="s">
         <v>7545</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G28" s="55" t="s">
-        <v>7641</v>
+        <v>7521</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7649</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18" t="s">
@@ -25046,26 +25044,26 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="51" t="s">
         <v>7546</v>
       </c>
       <c r="B29" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E29" s="54" t="s">
+      <c r="E29" s="51" t="s">
         <v>7546</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G29" s="55" t="s">
-        <v>7642</v>
+        <v>7521</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7650</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="18" t="s">
@@ -25084,26 +25082,26 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="51" t="s">
         <v>7547</v>
       </c>
       <c r="B30" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E30" s="54" t="s">
+      <c r="E30" s="51" t="s">
         <v>7547</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G30" s="55" t="s">
-        <v>7643</v>
+        <v>7521</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7651</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="18" t="s">
@@ -25122,26 +25120,26 @@
       <c r="M30" s="25"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="51" t="s">
         <v>7548</v>
       </c>
       <c r="B31" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E31" s="54" t="s">
+      <c r="E31" s="51" t="s">
         <v>7548</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G31" s="55" t="s">
-        <v>7644</v>
+        <v>7521</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7652</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18" t="s">
@@ -25160,26 +25158,26 @@
       <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="51" t="s">
         <v>7549</v>
       </c>
       <c r="B32" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E32" s="54" t="s">
+      <c r="E32" s="51" t="s">
         <v>7549</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>7645</v>
+        <v>7521</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7653</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18" t="s">
@@ -25198,26 +25196,26 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="51" t="s">
         <v>7550</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E33" s="54" t="s">
+      <c r="E33" s="51" t="s">
         <v>7550</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G33" s="55" t="s">
-        <v>7646</v>
+        <v>7521</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7654</v>
       </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18" t="s">
@@ -25236,26 +25234,26 @@
       <c r="M33" s="26"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="51" t="s">
         <v>7551</v>
       </c>
       <c r="B34" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E34" s="54" t="s">
+      <c r="E34" s="51" t="s">
         <v>7551</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G34" s="55" t="s">
-        <v>7647</v>
+        <v>7521</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7655</v>
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
@@ -25274,26 +25272,26 @@
       <c r="M34" s="22"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="51" t="s">
         <v>7552</v>
       </c>
       <c r="B35" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E35" s="54" t="s">
+      <c r="E35" s="51" t="s">
         <v>7552</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G35" s="55" t="s">
-        <v>7648</v>
+        <v>7521</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7656</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="18" t="s">
@@ -25312,26 +25310,26 @@
       <c r="M35" s="22"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="51" t="s">
         <v>7553</v>
       </c>
       <c r="B36" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E36" s="54" t="s">
+      <c r="E36" s="51" t="s">
         <v>7553</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G36" s="55" t="s">
-        <v>7649</v>
+        <v>7521</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7657</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="18" t="s">
@@ -25350,26 +25348,26 @@
       <c r="M36" s="22"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="51" t="s">
         <v>7554</v>
       </c>
       <c r="B37" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E37" s="54" t="s">
+      <c r="E37" s="51" t="s">
         <v>7554</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G37" s="55" t="s">
-        <v>7650</v>
+        <v>7521</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7658</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18" t="s">
@@ -25388,26 +25386,26 @@
       <c r="M37" s="22"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="51" t="s">
         <v>7555</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E38" s="54" t="s">
+      <c r="E38" s="51" t="s">
         <v>7555</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G38" s="55" t="s">
-        <v>7651</v>
+        <v>7521</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7659</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18" t="s">
@@ -25426,26 +25424,26 @@
       <c r="M38" s="22"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="51" t="s">
         <v>7556</v>
       </c>
       <c r="B39" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E39" s="54" t="s">
+      <c r="E39" s="51" t="s">
         <v>7556</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G39" s="55" t="s">
-        <v>7652</v>
+        <v>7521</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7660</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="18" t="s">
@@ -25464,26 +25462,26 @@
       <c r="M39" s="20"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="51" t="s">
         <v>7557</v>
       </c>
       <c r="B40" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E40" s="54" t="s">
+      <c r="E40" s="51" t="s">
         <v>7557</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G40" s="55" t="s">
-        <v>7653</v>
+        <v>7521</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7661</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
@@ -25502,26 +25500,26 @@
       <c r="M40" s="18"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="51" t="s">
         <v>7558</v>
       </c>
       <c r="B41" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E41" s="54" t="s">
+      <c r="E41" s="51" t="s">
         <v>7558</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G41" s="55" t="s">
-        <v>7654</v>
+        <v>7521</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7662</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="18" t="s">
@@ -25540,26 +25538,26 @@
       <c r="M41" s="24"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="51" t="s">
         <v>7559</v>
       </c>
       <c r="B42" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E42" s="54" t="s">
+      <c r="E42" s="51" t="s">
         <v>7559</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G42" s="55" t="s">
-        <v>7655</v>
+        <v>7521</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7663</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="18" t="s">
@@ -25578,26 +25576,26 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="54" t="s">
+      <c r="A43" s="51" t="s">
         <v>7560</v>
       </c>
       <c r="B43" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E43" s="54" t="s">
+      <c r="E43" s="51" t="s">
         <v>7560</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G43" s="55" t="s">
-        <v>7656</v>
+        <v>7521</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7664</v>
       </c>
       <c r="H43" s="18"/>
       <c r="I43" s="18" t="s">
@@ -25616,26 +25614,26 @@
       <c r="M43" s="18"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="51" t="s">
         <v>7561</v>
       </c>
       <c r="B44" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E44" s="54" t="s">
+      <c r="E44" s="51" t="s">
         <v>7561</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G44" s="55" t="s">
-        <v>7657</v>
+        <v>7521</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7665</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="18" t="s">
@@ -25654,26 +25652,26 @@
       <c r="M44" s="22"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="54" t="s">
+      <c r="A45" s="51" t="s">
         <v>7562</v>
       </c>
       <c r="B45" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="E45" s="51" t="s">
         <v>7562</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G45" s="55" t="s">
-        <v>7658</v>
+        <v>7521</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7666</v>
       </c>
       <c r="H45" s="18"/>
       <c r="I45" s="18" t="s">
@@ -25692,26 +25690,26 @@
       <c r="M45" s="18"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="51" t="s">
         <v>7563</v>
       </c>
       <c r="B46" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E46" s="54" t="s">
+      <c r="E46" s="51" t="s">
         <v>7563</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G46" s="55" t="s">
-        <v>7659</v>
+        <v>7521</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7667</v>
       </c>
       <c r="H46" s="18"/>
       <c r="I46" s="18" t="s">
@@ -25730,26 +25728,26 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="54" t="s">
+      <c r="A47" s="51" t="s">
         <v>7564</v>
       </c>
       <c r="B47" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C47" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="E47" s="51" t="s">
         <v>7564</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G47" s="55" t="s">
-        <v>7660</v>
+        <v>7521</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7668</v>
       </c>
       <c r="H47" s="18"/>
       <c r="I47" s="18" t="s">
@@ -25768,26 +25766,26 @@
       <c r="M47" s="18"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="54" t="s">
+      <c r="A48" s="51" t="s">
         <v>7565</v>
       </c>
       <c r="B48" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E48" s="54" t="s">
+      <c r="E48" s="51" t="s">
         <v>7565</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G48" s="55" t="s">
-        <v>7661</v>
+        <v>7521</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7669</v>
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="18" t="s">
@@ -25806,26 +25804,26 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="51" t="s">
         <v>7566</v>
       </c>
       <c r="B49" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E49" s="54" t="s">
+      <c r="E49" s="51" t="s">
         <v>7566</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G49" s="55" t="s">
-        <v>7662</v>
+        <v>7521</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7670</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18" t="s">
@@ -25844,26 +25842,26 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="51" t="s">
         <v>7567</v>
       </c>
       <c r="B50" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E50" s="54" t="s">
+      <c r="E50" s="51" t="s">
         <v>7567</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G50" s="55" t="s">
-        <v>7663</v>
+        <v>7521</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7671</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18" t="s">
@@ -25882,26 +25880,26 @@
       <c r="M50" s="18"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A51" s="54" t="s">
+      <c r="A51" s="51" t="s">
         <v>7568</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E51" s="54" t="s">
+      <c r="E51" s="51" t="s">
         <v>7568</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G51" s="55" t="s">
-        <v>7664</v>
+        <v>7521</v>
+      </c>
+      <c r="G51" t="s">
+        <v>7672</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="18" t="s">
@@ -25920,26 +25918,26 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="51" t="s">
         <v>7569</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E52" s="54" t="s">
+      <c r="E52" s="51" t="s">
         <v>7569</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G52" s="55" t="s">
-        <v>7665</v>
+        <v>7521</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7673</v>
       </c>
       <c r="H52" s="18"/>
       <c r="I52" s="18" t="s">
@@ -25958,26 +25956,26 @@
       <c r="M52" s="18"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A53" s="54" t="s">
+      <c r="A53" s="51" t="s">
         <v>7570</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C53" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E53" s="54" t="s">
+      <c r="E53" s="51" t="s">
         <v>7570</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G53" s="55" t="s">
-        <v>7666</v>
+        <v>7521</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7674</v>
       </c>
       <c r="H53" s="18"/>
       <c r="I53" s="18" t="s">
@@ -25996,26 +25994,26 @@
       <c r="M53" s="18"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="51" t="s">
         <v>7571</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E54" s="54" t="s">
+      <c r="E54" s="51" t="s">
         <v>7571</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G54" s="55" t="s">
-        <v>7667</v>
+        <v>7521</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7675</v>
       </c>
       <c r="H54" s="18"/>
       <c r="I54" s="18" t="s">
@@ -26034,26 +26032,26 @@
       <c r="M54" s="25"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="51" t="s">
         <v>7572</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E55" s="54" t="s">
+      <c r="E55" s="51" t="s">
         <v>7572</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G55" s="55" t="s">
-        <v>7668</v>
+        <v>7521</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7676</v>
       </c>
       <c r="H55" s="18"/>
       <c r="I55" s="18" t="s">
@@ -26072,26 +26070,26 @@
       <c r="M55" s="25"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="51" t="s">
         <v>7573</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E56" s="54" t="s">
+      <c r="E56" s="51" t="s">
         <v>7573</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G56" s="55" t="s">
-        <v>7669</v>
+        <v>7521</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7677</v>
       </c>
       <c r="H56" s="18"/>
       <c r="I56" s="18" t="s">
@@ -26110,26 +26108,26 @@
       <c r="M56" s="18"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="51" t="s">
         <v>7574</v>
       </c>
       <c r="B57" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E57" s="54" t="s">
+      <c r="E57" s="51" t="s">
         <v>7574</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G57" s="55" t="s">
-        <v>7670</v>
+        <v>7521</v>
+      </c>
+      <c r="G57" t="s">
+        <v>7678</v>
       </c>
       <c r="H57" s="18"/>
       <c r="I57" s="18" t="s">
@@ -26148,26 +26146,26 @@
       <c r="M57" s="26"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="51" t="s">
         <v>7575</v>
       </c>
       <c r="B58" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E58" s="54" t="s">
+      <c r="E58" s="51" t="s">
         <v>7575</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G58" s="55" t="s">
-        <v>7671</v>
+        <v>7521</v>
+      </c>
+      <c r="G58" t="s">
+        <v>7679</v>
       </c>
       <c r="H58" s="18"/>
       <c r="I58" s="18" t="s">
@@ -26186,26 +26184,26 @@
       <c r="M58" s="22"/>
     </row>
     <row r="59" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="51" t="s">
         <v>7576</v>
       </c>
       <c r="B59" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E59" s="54" t="s">
+      <c r="E59" s="51" t="s">
         <v>7576</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G59" s="55" t="s">
-        <v>7672</v>
+        <v>7521</v>
+      </c>
+      <c r="G59" t="s">
+        <v>7680</v>
       </c>
       <c r="H59" s="18"/>
       <c r="I59" s="18" t="s">
@@ -26224,26 +26222,26 @@
       <c r="M59" s="22"/>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="51" t="s">
         <v>7577</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E60" s="54" t="s">
+      <c r="E60" s="51" t="s">
         <v>7577</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G60" s="55" t="s">
-        <v>7673</v>
+        <v>7521</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7681</v>
       </c>
       <c r="H60" s="18"/>
       <c r="I60" s="18" t="s">
@@ -26262,26 +26260,26 @@
       <c r="M60" s="22"/>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="51" t="s">
         <v>7578</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>44</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E61" s="54" t="s">
+      <c r="E61" s="51" t="s">
         <v>7578</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G61" s="55" t="s">
-        <v>7674</v>
+        <v>7521</v>
+      </c>
+      <c r="G61" t="s">
+        <v>7682</v>
       </c>
       <c r="H61" s="18"/>
       <c r="I61" s="18" t="s">
@@ -26300,26 +26298,26 @@
       <c r="M61" s="22"/>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="51" t="s">
         <v>7579</v>
       </c>
       <c r="B62" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E62" s="54" t="s">
+      <c r="E62" s="51" t="s">
         <v>7579</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G62" s="55" t="s">
-        <v>7675</v>
+        <v>7521</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7683</v>
       </c>
       <c r="H62" s="18"/>
       <c r="I62" s="18" t="s">
@@ -26338,26 +26336,26 @@
       <c r="M62" s="22"/>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A63" s="54" t="s">
+      <c r="A63" s="51" t="s">
         <v>7580</v>
       </c>
       <c r="B63" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E63" s="54" t="s">
+      <c r="E63" s="51" t="s">
         <v>7580</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G63" s="55" t="s">
-        <v>7676</v>
+        <v>7521</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7684</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="18" t="s">
@@ -26376,26 +26374,26 @@
       <c r="M63" s="20"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A64" s="54" t="s">
+      <c r="A64" s="51" t="s">
         <v>7581</v>
       </c>
       <c r="B64" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E64" s="54" t="s">
+      <c r="E64" s="51" t="s">
         <v>7581</v>
       </c>
       <c r="F64" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G64" s="55" t="s">
-        <v>7677</v>
+        <v>7521</v>
+      </c>
+      <c r="G64" t="s">
+        <v>7685</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="18" t="s">
@@ -26414,26 +26412,26 @@
       <c r="M64" s="18"/>
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A65" s="54" t="s">
+      <c r="A65" s="51" t="s">
         <v>7582</v>
       </c>
       <c r="B65" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E65" s="54" t="s">
+      <c r="E65" s="51" t="s">
         <v>7582</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G65" s="55" t="s">
-        <v>7678</v>
+        <v>7521</v>
+      </c>
+      <c r="G65" t="s">
+        <v>7686</v>
       </c>
       <c r="H65" s="18"/>
       <c r="I65" s="18" t="s">
@@ -26452,26 +26450,26 @@
       <c r="M65" s="24"/>
     </row>
     <row r="66" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="51" t="s">
         <v>7583</v>
       </c>
       <c r="B66" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E66" s="54" t="s">
+      <c r="E66" s="51" t="s">
         <v>7583</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G66" s="55" t="s">
-        <v>7679</v>
+        <v>7521</v>
+      </c>
+      <c r="G66" t="s">
+        <v>7687</v>
       </c>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
@@ -26490,26 +26488,26 @@
       <c r="M66" s="18"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="51" t="s">
         <v>7584</v>
       </c>
       <c r="B67" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E67" s="54" t="s">
+      <c r="E67" s="51" t="s">
         <v>7584</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G67" s="55" t="s">
-        <v>7680</v>
+        <v>7521</v>
+      </c>
+      <c r="G67" t="s">
+        <v>7688</v>
       </c>
       <c r="H67" s="18"/>
       <c r="I67" s="18" t="s">
@@ -26528,26 +26526,26 @@
       <c r="M67" s="18"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A68" s="54" t="s">
+      <c r="A68" s="51" t="s">
         <v>7585</v>
       </c>
       <c r="B68" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="51" t="s">
         <v>7585</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G68" s="55" t="s">
-        <v>7681</v>
+        <v>7521</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7689</v>
       </c>
       <c r="H68" s="18"/>
       <c r="I68" s="18" t="s">
@@ -26566,26 +26564,26 @@
       <c r="M68" s="22"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A69" s="54" t="s">
+      <c r="A69" s="51" t="s">
         <v>7586</v>
       </c>
       <c r="B69" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E69" s="54" t="s">
+      <c r="E69" s="51" t="s">
         <v>7586</v>
       </c>
       <c r="F69" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G69" s="55" t="s">
-        <v>7682</v>
+        <v>7521</v>
+      </c>
+      <c r="G69" t="s">
+        <v>7690</v>
       </c>
       <c r="H69" s="18"/>
       <c r="I69" s="18" t="s">
@@ -26604,26 +26602,26 @@
       <c r="M69" s="18"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="51" t="s">
         <v>7587</v>
       </c>
       <c r="B70" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E70" s="54" t="s">
+      <c r="E70" s="51" t="s">
         <v>7587</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G70" s="55" t="s">
-        <v>7683</v>
+        <v>7521</v>
+      </c>
+      <c r="G70" t="s">
+        <v>7691</v>
       </c>
       <c r="H70" s="18"/>
       <c r="I70" s="18" t="s">
@@ -26642,26 +26640,26 @@
       <c r="M70" s="18"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A71" s="54" t="s">
+      <c r="A71" s="51" t="s">
         <v>7588</v>
       </c>
       <c r="B71" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E71" s="54" t="s">
+      <c r="E71" s="51" t="s">
         <v>7588</v>
       </c>
       <c r="F71" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G71" s="55" t="s">
-        <v>7684</v>
+        <v>7521</v>
+      </c>
+      <c r="G71" t="s">
+        <v>7692</v>
       </c>
       <c r="H71" s="18"/>
       <c r="I71" s="18" t="s">
@@ -26680,26 +26678,26 @@
       <c r="M71" s="18"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A72" s="54" t="s">
+      <c r="A72" s="51" t="s">
         <v>7589</v>
       </c>
       <c r="B72" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C72" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E72" s="54" t="s">
+      <c r="E72" s="51" t="s">
         <v>7589</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G72" s="55" t="s">
-        <v>7685</v>
+        <v>7521</v>
+      </c>
+      <c r="G72" t="s">
+        <v>7693</v>
       </c>
       <c r="H72" s="18"/>
       <c r="I72" s="18" t="s">
@@ -26718,26 +26716,26 @@
       <c r="M72" s="18"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A73" s="54" t="s">
+      <c r="A73" s="51" t="s">
         <v>7590</v>
       </c>
       <c r="B73" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E73" s="54" t="s">
+      <c r="E73" s="51" t="s">
         <v>7590</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G73" s="55" t="s">
-        <v>7686</v>
+        <v>7521</v>
+      </c>
+      <c r="G73" t="s">
+        <v>7694</v>
       </c>
       <c r="H73" s="18"/>
       <c r="I73" s="18" t="s">
@@ -26756,26 +26754,26 @@
       <c r="M73" s="18"/>
     </row>
     <row r="74" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A74" s="54" t="s">
+      <c r="A74" s="51" t="s">
         <v>7591</v>
       </c>
       <c r="B74" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E74" s="54" t="s">
+      <c r="E74" s="51" t="s">
         <v>7591</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G74" s="55" t="s">
-        <v>7687</v>
+        <v>7521</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7695</v>
       </c>
       <c r="H74" s="18"/>
       <c r="I74" s="18" t="s">
@@ -26794,26 +26792,26 @@
       <c r="M74" s="18"/>
     </row>
     <row r="75" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A75" s="54" t="s">
+      <c r="A75" s="51" t="s">
         <v>7592</v>
       </c>
       <c r="B75" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E75" s="54" t="s">
+      <c r="E75" s="51" t="s">
         <v>7592</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G75" s="55" t="s">
-        <v>7688</v>
+        <v>7521</v>
+      </c>
+      <c r="G75" t="s">
+        <v>7696</v>
       </c>
       <c r="H75" s="18"/>
       <c r="I75" s="18" t="s">
@@ -26832,26 +26830,26 @@
       <c r="M75" s="18"/>
     </row>
     <row r="76" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A76" s="54" t="s">
+      <c r="A76" s="51" t="s">
         <v>7593</v>
       </c>
       <c r="B76" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E76" s="54" t="s">
+      <c r="E76" s="51" t="s">
         <v>7593</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G76" s="55" t="s">
-        <v>7689</v>
+        <v>7521</v>
+      </c>
+      <c r="G76" t="s">
+        <v>7697</v>
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="18" t="s">
@@ -26870,26 +26868,26 @@
       <c r="M76" s="18"/>
     </row>
     <row r="77" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A77" s="54" t="s">
+      <c r="A77" s="51" t="s">
         <v>7594</v>
       </c>
       <c r="B77" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E77" s="54" t="s">
+      <c r="E77" s="51" t="s">
         <v>7594</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G77" s="55" t="s">
-        <v>7690</v>
+        <v>7521</v>
+      </c>
+      <c r="G77" t="s">
+        <v>7698</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="18" t="s">
@@ -26908,26 +26906,26 @@
       <c r="M77" s="18"/>
     </row>
     <row r="78" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A78" s="54" t="s">
+      <c r="A78" s="51" t="s">
         <v>7595</v>
       </c>
       <c r="B78" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E78" s="54" t="s">
+      <c r="E78" s="51" t="s">
         <v>7595</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G78" s="55" t="s">
-        <v>7691</v>
+        <v>7521</v>
+      </c>
+      <c r="G78" t="s">
+        <v>7699</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="18" t="s">
@@ -26946,26 +26944,26 @@
       <c r="M78" s="25"/>
     </row>
     <row r="79" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A79" s="54" t="s">
+      <c r="A79" s="51" t="s">
         <v>7596</v>
       </c>
       <c r="B79" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E79" s="54" t="s">
+      <c r="E79" s="51" t="s">
         <v>7596</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G79" s="55" t="s">
-        <v>7692</v>
+        <v>7521</v>
+      </c>
+      <c r="G79" t="s">
+        <v>7700</v>
       </c>
       <c r="H79" s="18"/>
       <c r="I79" s="18" t="s">
@@ -26984,26 +26982,26 @@
       <c r="M79" s="25"/>
     </row>
     <row r="80" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A80" s="54" t="s">
+      <c r="A80" s="51" t="s">
         <v>7597</v>
       </c>
       <c r="B80" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C80" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D80" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E80" s="54" t="s">
+      <c r="E80" s="51" t="s">
         <v>7597</v>
       </c>
       <c r="F80" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G80" s="55" t="s">
-        <v>7693</v>
+        <v>7521</v>
+      </c>
+      <c r="G80" t="s">
+        <v>7701</v>
       </c>
       <c r="H80" s="18"/>
       <c r="I80" s="18" t="s">
@@ -27022,26 +27020,26 @@
       <c r="M80" s="18"/>
     </row>
     <row r="81" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A81" s="54" t="s">
+      <c r="A81" s="51" t="s">
         <v>7598</v>
       </c>
       <c r="B81" s="43" t="s">
         <v>47</v>
       </c>
       <c r="C81" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E81" s="54" t="s">
+      <c r="E81" s="51" t="s">
         <v>7598</v>
       </c>
       <c r="F81" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G81" s="55" t="s">
-        <v>7694</v>
+        <v>7521</v>
+      </c>
+      <c r="G81" t="s">
+        <v>7702</v>
       </c>
       <c r="H81" s="18"/>
       <c r="I81" s="18" t="s">
@@ -27060,26 +27058,26 @@
       <c r="M81" s="26"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A82" s="54" t="s">
+      <c r="A82" s="51" t="s">
         <v>7599</v>
       </c>
       <c r="B82" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C82" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D82" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E82" s="54" t="s">
+      <c r="E82" s="51" t="s">
         <v>7599</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G82" s="55" t="s">
-        <v>7695</v>
+        <v>7521</v>
+      </c>
+      <c r="G82" t="s">
+        <v>7703</v>
       </c>
       <c r="H82" s="18"/>
       <c r="I82" s="18" t="s">
@@ -27098,26 +27096,26 @@
       <c r="M82" s="22"/>
     </row>
     <row r="83" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A83" s="54" t="s">
+      <c r="A83" s="51" t="s">
         <v>7600</v>
       </c>
       <c r="B83" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E83" s="54" t="s">
+      <c r="E83" s="51" t="s">
         <v>7600</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G83" s="55" t="s">
-        <v>7696</v>
+        <v>7521</v>
+      </c>
+      <c r="G83" t="s">
+        <v>7704</v>
       </c>
       <c r="H83" s="18"/>
       <c r="I83" s="18" t="s">
@@ -27136,26 +27134,26 @@
       <c r="M83" s="22"/>
     </row>
     <row r="84" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A84" s="54" t="s">
+      <c r="A84" s="51" t="s">
         <v>7601</v>
       </c>
       <c r="B84" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D84" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E84" s="54" t="s">
+      <c r="E84" s="51" t="s">
         <v>7601</v>
       </c>
       <c r="F84" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G84" s="55" t="s">
-        <v>7697</v>
+        <v>7521</v>
+      </c>
+      <c r="G84" t="s">
+        <v>7705</v>
       </c>
       <c r="H84" s="18"/>
       <c r="I84" s="18" t="s">
@@ -27174,26 +27172,26 @@
       <c r="M84" s="22"/>
     </row>
     <row r="85" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A85" s="54" t="s">
+      <c r="A85" s="51" t="s">
         <v>7602</v>
       </c>
       <c r="B85" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E85" s="54" t="s">
+      <c r="E85" s="51" t="s">
         <v>7602</v>
       </c>
       <c r="F85" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G85" s="55" t="s">
-        <v>7698</v>
+        <v>7521</v>
+      </c>
+      <c r="G85" t="s">
+        <v>7706</v>
       </c>
       <c r="H85" s="18"/>
       <c r="I85" s="18" t="s">
@@ -27212,26 +27210,26 @@
       <c r="M85" s="22"/>
     </row>
     <row r="86" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A86" s="54" t="s">
+      <c r="A86" s="51" t="s">
         <v>7603</v>
       </c>
       <c r="B86" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D86" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E86" s="54" t="s">
+      <c r="E86" s="51" t="s">
         <v>7603</v>
       </c>
       <c r="F86" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G86" s="55" t="s">
-        <v>7699</v>
+        <v>7521</v>
+      </c>
+      <c r="G86" t="s">
+        <v>7707</v>
       </c>
       <c r="H86" s="18"/>
       <c r="I86" s="18" t="s">
@@ -27250,26 +27248,26 @@
       <c r="M86" s="22"/>
     </row>
     <row r="87" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A87" s="54" t="s">
+      <c r="A87" s="51" t="s">
         <v>7604</v>
       </c>
       <c r="B87" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E87" s="54" t="s">
+      <c r="E87" s="51" t="s">
         <v>7604</v>
       </c>
       <c r="F87" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G87" s="55" t="s">
-        <v>7700</v>
+        <v>7521</v>
+      </c>
+      <c r="G87" t="s">
+        <v>7708</v>
       </c>
       <c r="H87" s="18"/>
       <c r="I87" s="18" t="s">
@@ -27288,26 +27286,26 @@
       <c r="M87" s="20"/>
     </row>
     <row r="88" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A88" s="54" t="s">
+      <c r="A88" s="51" t="s">
         <v>7605</v>
       </c>
       <c r="B88" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E88" s="54" t="s">
+      <c r="E88" s="51" t="s">
         <v>7605</v>
       </c>
       <c r="F88" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G88" s="55" t="s">
-        <v>7701</v>
+        <v>7521</v>
+      </c>
+      <c r="G88" t="s">
+        <v>7709</v>
       </c>
       <c r="H88" s="18"/>
       <c r="I88" s="18" t="s">
@@ -27326,26 +27324,26 @@
       <c r="M88" s="18"/>
     </row>
     <row r="89" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A89" s="54" t="s">
+      <c r="A89" s="51" t="s">
         <v>7606</v>
       </c>
       <c r="B89" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D89" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E89" s="54" t="s">
+      <c r="E89" s="51" t="s">
         <v>7606</v>
       </c>
       <c r="F89" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G89" s="55" t="s">
-        <v>7702</v>
+        <v>7521</v>
+      </c>
+      <c r="G89" t="s">
+        <v>7710</v>
       </c>
       <c r="H89" s="18"/>
       <c r="I89" s="18" t="s">
@@ -27364,26 +27362,26 @@
       <c r="M89" s="24"/>
     </row>
     <row r="90" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A90" s="54" t="s">
+      <c r="A90" s="51" t="s">
         <v>7607</v>
       </c>
       <c r="B90" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E90" s="54" t="s">
+      <c r="E90" s="51" t="s">
         <v>7607</v>
       </c>
       <c r="F90" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G90" s="55" t="s">
-        <v>7703</v>
+        <v>7521</v>
+      </c>
+      <c r="G90" t="s">
+        <v>7711</v>
       </c>
       <c r="H90" s="18"/>
       <c r="I90" s="18" t="s">
@@ -27402,26 +27400,26 @@
       <c r="M90" s="18"/>
     </row>
     <row r="91" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A91" s="54" t="s">
+      <c r="A91" s="51" t="s">
         <v>7608</v>
       </c>
       <c r="B91" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D91" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E91" s="54" t="s">
+      <c r="E91" s="51" t="s">
         <v>7608</v>
       </c>
       <c r="F91" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G91" s="55" t="s">
-        <v>7704</v>
+        <v>7521</v>
+      </c>
+      <c r="G91" t="s">
+        <v>7712</v>
       </c>
       <c r="H91" s="18"/>
       <c r="I91" s="18" t="s">
@@ -27440,26 +27438,26 @@
       <c r="M91" s="18"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A92" s="54" t="s">
+      <c r="A92" s="51" t="s">
         <v>7609</v>
       </c>
       <c r="B92" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C92" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D92" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E92" s="54" t="s">
+      <c r="E92" s="51" t="s">
         <v>7609</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G92" s="55" t="s">
-        <v>7705</v>
+        <v>7521</v>
+      </c>
+      <c r="G92" t="s">
+        <v>7713</v>
       </c>
       <c r="H92" s="18"/>
       <c r="I92" s="18" t="s">
@@ -27478,26 +27476,26 @@
       <c r="M92" s="22"/>
     </row>
     <row r="93" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A93" s="54" t="s">
+      <c r="A93" s="51" t="s">
         <v>7610</v>
       </c>
       <c r="B93" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C93" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D93" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E93" s="54" t="s">
+      <c r="E93" s="51" t="s">
         <v>7610</v>
       </c>
       <c r="F93" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G93" s="55" t="s">
-        <v>7706</v>
+        <v>7521</v>
+      </c>
+      <c r="G93" t="s">
+        <v>7714</v>
       </c>
       <c r="H93" s="18"/>
       <c r="I93" s="18" t="s">
@@ -27516,26 +27514,26 @@
       <c r="M93" s="18"/>
     </row>
     <row r="94" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A94" s="54" t="s">
+      <c r="A94" s="51" t="s">
         <v>7611</v>
       </c>
       <c r="B94" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C94" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D94" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E94" s="54" t="s">
+      <c r="E94" s="51" t="s">
         <v>7611</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G94" s="55" t="s">
-        <v>7707</v>
+        <v>7521</v>
+      </c>
+      <c r="G94" t="s">
+        <v>7715</v>
       </c>
       <c r="H94" s="18"/>
       <c r="I94" s="18" t="s">
@@ -27554,26 +27552,26 @@
       <c r="M94" s="18"/>
     </row>
     <row r="95" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A95" s="54" t="s">
+      <c r="A95" s="51" t="s">
         <v>7612</v>
       </c>
       <c r="B95" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C95" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D95" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E95" s="54" t="s">
+      <c r="E95" s="51" t="s">
         <v>7612</v>
       </c>
       <c r="F95" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G95" s="55" t="s">
-        <v>7708</v>
+        <v>7521</v>
+      </c>
+      <c r="G95" t="s">
+        <v>7716</v>
       </c>
       <c r="H95" s="18"/>
       <c r="I95" s="18" t="s">
@@ -27592,26 +27590,26 @@
       <c r="M95" s="18"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A96" s="54" t="s">
+      <c r="A96" s="51" t="s">
         <v>7613</v>
       </c>
       <c r="B96" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C96" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D96" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E96" s="54" t="s">
+      <c r="E96" s="51" t="s">
         <v>7613</v>
       </c>
       <c r="F96" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G96" s="55" t="s">
-        <v>7709</v>
+        <v>7521</v>
+      </c>
+      <c r="G96" t="s">
+        <v>7717</v>
       </c>
       <c r="H96" s="18"/>
       <c r="I96" s="18" t="s">
@@ -27630,26 +27628,26 @@
       <c r="M96" s="18"/>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A97" s="54" t="s">
+      <c r="A97" s="51" t="s">
         <v>7614</v>
       </c>
       <c r="B97" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C97" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D97" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E97" s="54" t="s">
+      <c r="E97" s="51" t="s">
         <v>7614</v>
       </c>
       <c r="F97" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G97" s="55" t="s">
-        <v>7710</v>
+        <v>7521</v>
+      </c>
+      <c r="G97" t="s">
+        <v>7718</v>
       </c>
       <c r="H97" s="18"/>
       <c r="I97" s="18" t="s">
@@ -27668,26 +27666,26 @@
       <c r="M97" s="18"/>
     </row>
     <row r="98" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A98" s="54" t="s">
+      <c r="A98" s="51" t="s">
         <v>7615</v>
       </c>
       <c r="B98" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C98" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D98" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E98" s="54" t="s">
+      <c r="E98" s="51" t="s">
         <v>7615</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G98" s="55" t="s">
-        <v>7711</v>
+        <v>7521</v>
+      </c>
+      <c r="G98" t="s">
+        <v>7719</v>
       </c>
       <c r="H98" s="18"/>
       <c r="I98" s="18" t="s">
@@ -27706,26 +27704,26 @@
       <c r="M98" s="18"/>
     </row>
     <row r="99" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A99" s="54" t="s">
+      <c r="A99" s="51" t="s">
         <v>7616</v>
       </c>
       <c r="B99" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C99" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D99" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E99" s="54" t="s">
+      <c r="E99" s="51" t="s">
         <v>7616</v>
       </c>
       <c r="F99" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G99" s="55" t="s">
-        <v>7712</v>
+        <v>7521</v>
+      </c>
+      <c r="G99" t="s">
+        <v>7720</v>
       </c>
       <c r="H99" s="18"/>
       <c r="I99" s="18" t="s">
@@ -27744,26 +27742,26 @@
       <c r="M99" s="18"/>
     </row>
     <row r="100" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A100" s="54" t="s">
+      <c r="A100" s="51" t="s">
         <v>7617</v>
       </c>
       <c r="B100" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C100" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D100" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E100" s="54" t="s">
+      <c r="E100" s="51" t="s">
         <v>7617</v>
       </c>
       <c r="F100" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G100" s="55" t="s">
-        <v>7713</v>
+        <v>7521</v>
+      </c>
+      <c r="G100" t="s">
+        <v>7721</v>
       </c>
       <c r="H100" s="18"/>
       <c r="I100" s="18" t="s">
@@ -27782,26 +27780,26 @@
       <c r="M100" s="18"/>
     </row>
     <row r="101" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A101" s="54" t="s">
+      <c r="A101" s="51" t="s">
         <v>7618</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C101" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D101" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E101" s="54" t="s">
+      <c r="E101" s="51" t="s">
         <v>7618</v>
       </c>
       <c r="F101" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G101" s="55" t="s">
-        <v>7714</v>
+        <v>7521</v>
+      </c>
+      <c r="G101" t="s">
+        <v>7722</v>
       </c>
       <c r="H101" s="18"/>
       <c r="I101" s="18" t="s">
@@ -27820,26 +27818,26 @@
       <c r="M101" s="18"/>
     </row>
     <row r="102" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A102" s="54" t="s">
+      <c r="A102" s="51" t="s">
         <v>7619</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C102" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D102" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E102" s="54" t="s">
+      <c r="E102" s="51" t="s">
         <v>7619</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G102" s="55" t="s">
-        <v>7715</v>
+        <v>7521</v>
+      </c>
+      <c r="G102" t="s">
+        <v>7723</v>
       </c>
       <c r="H102" s="18"/>
       <c r="I102" s="18" t="s">
@@ -27858,26 +27856,26 @@
       <c r="M102" s="25"/>
     </row>
     <row r="103" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A103" s="54" t="s">
+      <c r="A103" s="51" t="s">
         <v>7620</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C103" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D103" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E103" s="54" t="s">
+      <c r="E103" s="51" t="s">
         <v>7620</v>
       </c>
       <c r="F103" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G103" s="55" t="s">
-        <v>7716</v>
+        <v>7521</v>
+      </c>
+      <c r="G103" t="s">
+        <v>7724</v>
       </c>
       <c r="H103" s="18"/>
       <c r="I103" s="18" t="s">
@@ -27896,26 +27894,26 @@
       <c r="M103" s="25"/>
     </row>
     <row r="104" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A104" s="54" t="s">
+      <c r="A104" s="51" t="s">
         <v>7621</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C104" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D104" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E104" s="54" t="s">
+      <c r="E104" s="51" t="s">
         <v>7621</v>
       </c>
       <c r="F104" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G104" s="55" t="s">
-        <v>7717</v>
+        <v>7521</v>
+      </c>
+      <c r="G104" t="s">
+        <v>7725</v>
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="18" t="s">
@@ -27934,26 +27932,26 @@
       <c r="M104" s="18"/>
     </row>
     <row r="105" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A105" s="54" t="s">
+      <c r="A105" s="51" t="s">
         <v>7622</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C105" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D105" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E105" s="54" t="s">
+      <c r="E105" s="51" t="s">
         <v>7622</v>
       </c>
       <c r="F105" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G105" s="55" t="s">
-        <v>7718</v>
+        <v>7521</v>
+      </c>
+      <c r="G105" t="s">
+        <v>7726</v>
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="18" t="s">
@@ -27972,26 +27970,26 @@
       <c r="M105" s="26"/>
     </row>
     <row r="106" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A106" s="54" t="s">
+      <c r="A106" s="51" t="s">
         <v>7623</v>
       </c>
       <c r="B106" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C106" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D106" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E106" s="54" t="s">
+      <c r="E106" s="51" t="s">
         <v>7623</v>
       </c>
       <c r="F106" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G106" s="55" t="s">
-        <v>7719</v>
+        <v>7521</v>
+      </c>
+      <c r="G106" t="s">
+        <v>7727</v>
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="18" t="s">
@@ -28010,26 +28008,26 @@
       <c r="M106" s="22"/>
     </row>
     <row r="107" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A107" s="54" t="s">
+      <c r="A107" s="51" t="s">
         <v>7624</v>
       </c>
       <c r="B107" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C107" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D107" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E107" s="54" t="s">
+      <c r="E107" s="51" t="s">
         <v>7624</v>
       </c>
       <c r="F107" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G107" s="55" t="s">
-        <v>7720</v>
+        <v>7521</v>
+      </c>
+      <c r="G107" t="s">
+        <v>7728</v>
       </c>
       <c r="H107" s="18"/>
       <c r="I107" s="18" t="s">
@@ -28048,26 +28046,26 @@
       <c r="M107" s="22"/>
     </row>
     <row r="108" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A108" s="54" t="s">
+      <c r="A108" s="51" t="s">
         <v>7625</v>
       </c>
       <c r="B108" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D108" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E108" s="54" t="s">
+      <c r="E108" s="51" t="s">
         <v>7625</v>
       </c>
       <c r="F108" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G108" s="55" t="s">
-        <v>7721</v>
+        <v>7521</v>
+      </c>
+      <c r="G108" t="s">
+        <v>7729</v>
       </c>
       <c r="H108" s="18"/>
       <c r="I108" s="18" t="s">
@@ -28086,26 +28084,26 @@
       <c r="M108" s="22"/>
     </row>
     <row r="109" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A109" s="54" t="s">
+      <c r="A109" s="51" t="s">
         <v>7626</v>
       </c>
       <c r="B109" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C109" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D109" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E109" s="54" t="s">
+      <c r="E109" s="51" t="s">
         <v>7626</v>
       </c>
       <c r="F109" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G109" s="55" t="s">
-        <v>7722</v>
+        <v>7521</v>
+      </c>
+      <c r="G109" t="s">
+        <v>7730</v>
       </c>
       <c r="H109" s="18"/>
       <c r="I109" s="18" t="s">
@@ -28124,26 +28122,26 @@
       <c r="M109" s="22"/>
     </row>
     <row r="110" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A110" s="54" t="s">
+      <c r="A110" s="51" t="s">
         <v>7627</v>
       </c>
       <c r="B110" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C110" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D110" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E110" s="54" t="s">
+      <c r="E110" s="51" t="s">
         <v>7627</v>
       </c>
       <c r="F110" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G110" s="55" t="s">
-        <v>7723</v>
+        <v>7521</v>
+      </c>
+      <c r="G110" t="s">
+        <v>7731</v>
       </c>
       <c r="H110" s="18"/>
       <c r="I110" s="18" t="s">
@@ -28162,26 +28160,26 @@
       <c r="M110" s="22"/>
     </row>
     <row r="111" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A111" s="54" t="s">
+      <c r="A111" s="51" t="s">
         <v>7628</v>
       </c>
       <c r="B111" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C111" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D111" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E111" s="54" t="s">
+      <c r="E111" s="51" t="s">
         <v>7628</v>
       </c>
       <c r="F111" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G111" s="55" t="s">
-        <v>7724</v>
+        <v>7521</v>
+      </c>
+      <c r="G111" t="s">
+        <v>7732</v>
       </c>
       <c r="H111" s="18"/>
       <c r="I111" s="18" t="s">
@@ -28200,26 +28198,26 @@
       <c r="M111" s="20"/>
     </row>
     <row r="112" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A112" s="54" t="s">
+      <c r="A112" s="51" t="s">
         <v>7629</v>
       </c>
       <c r="B112" s="43" t="s">
         <v>55</v>
       </c>
       <c r="C112" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D112" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E112" s="54" t="s">
+      <c r="E112" s="51" t="s">
         <v>7629</v>
       </c>
       <c r="F112" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G112" s="55" t="s">
-        <v>7725</v>
+        <v>7521</v>
+      </c>
+      <c r="G112" t="s">
+        <v>7733</v>
       </c>
       <c r="H112" s="18"/>
       <c r="I112" s="18" t="s">
@@ -28238,26 +28236,26 @@
       <c r="M112" s="18"/>
     </row>
     <row r="113" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A113" s="54" t="s">
+      <c r="A113" s="51" t="s">
         <v>7630</v>
       </c>
       <c r="B113" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C113" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D113" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E113" s="54" t="s">
+      <c r="E113" s="51" t="s">
         <v>7630</v>
       </c>
       <c r="F113" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G113" s="55" t="s">
-        <v>7726</v>
+        <v>7521</v>
+      </c>
+      <c r="G113" t="s">
+        <v>7734</v>
       </c>
       <c r="H113" s="18"/>
       <c r="I113" s="18" t="s">
@@ -28276,26 +28274,26 @@
       <c r="M113" s="24"/>
     </row>
     <row r="114" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A114" s="54" t="s">
+      <c r="A114" s="51" t="s">
         <v>7631</v>
       </c>
       <c r="B114" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C114" s="43" t="s">
-        <v>7733</v>
+        <v>7633</v>
       </c>
       <c r="D114" s="18" t="s">
         <v>7445</v>
       </c>
-      <c r="E114" s="54" t="s">
+      <c r="E114" s="51" t="s">
         <v>7631</v>
       </c>
       <c r="F114" s="18" t="s">
-        <v>7529</v>
-      </c>
-      <c r="G114" s="55" t="s">
-        <v>7727</v>
+        <v>7521</v>
+      </c>
+      <c r="G114" t="s">
+        <v>7735</v>
       </c>
       <c r="H114" s="18"/>
       <c r="I114" s="18" t="s">
@@ -28314,7 +28312,7 @@
       <c r="M114" s="18"/>
     </row>
     <row r="115" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A115" s="54"/>
+      <c r="A115" s="51"/>
       <c r="B115" s="18"/>
       <c r="C115" s="18"/>
       <c r="D115" s="21"/>
@@ -28336,7 +28334,7 @@
       <c r="M115" s="18"/>
     </row>
     <row r="116" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A116" s="54"/>
+      <c r="A116" s="51"/>
       <c r="B116" s="18"/>
       <c r="C116" s="18"/>
       <c r="D116" s="21"/>
@@ -28358,7 +28356,7 @@
       <c r="M116" s="22"/>
     </row>
     <row r="117" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A117" s="54"/>
+      <c r="A117" s="51"/>
       <c r="B117" s="18"/>
       <c r="C117" s="18"/>
       <c r="D117" s="21"/>
@@ -28380,7 +28378,7 @@
       <c r="M117" s="18"/>
     </row>
     <row r="118" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A118" s="54"/>
+      <c r="A118" s="51"/>
       <c r="B118" s="18"/>
       <c r="C118" s="18"/>
       <c r="D118" s="18"/>
@@ -28402,7 +28400,7 @@
       <c r="M118" s="18"/>
     </row>
     <row r="119" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A119" s="54"/>
+      <c r="A119" s="51"/>
       <c r="B119" s="18"/>
       <c r="C119" s="18"/>
       <c r="D119" s="18"/>
@@ -28424,7 +28422,7 @@
       <c r="M119" s="18"/>
     </row>
     <row r="120" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A120" s="54"/>
+      <c r="A120" s="51"/>
       <c r="B120" s="18"/>
       <c r="C120" s="18"/>
       <c r="D120" s="21"/>
@@ -28446,7 +28444,7 @@
       <c r="M120" s="18"/>
     </row>
     <row r="121" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A121" s="54"/>
+      <c r="A121" s="51"/>
       <c r="B121" s="18"/>
       <c r="C121" s="18"/>
       <c r="D121" s="21"/>
@@ -28468,7 +28466,7 @@
       <c r="M121" s="18"/>
     </row>
     <row r="122" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A122" s="54"/>
+      <c r="A122" s="51"/>
       <c r="B122" s="18"/>
       <c r="C122" s="18"/>
       <c r="D122" s="18"/>
@@ -28490,7 +28488,7 @@
       <c r="M122" s="18"/>
     </row>
     <row r="123" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A123" s="54"/>
+      <c r="A123" s="51"/>
       <c r="B123" s="18"/>
       <c r="C123" s="18"/>
       <c r="D123" s="21"/>
@@ -28512,7 +28510,7 @@
       <c r="M123" s="18"/>
     </row>
     <row r="124" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A124" s="54"/>
+      <c r="A124" s="51"/>
       <c r="B124" s="18"/>
       <c r="C124" s="18"/>
       <c r="D124" s="21"/>
@@ -28534,7 +28532,7 @@
       <c r="M124" s="18"/>
     </row>
     <row r="125" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A125" s="54"/>
+      <c r="A125" s="51"/>
       <c r="B125" s="18"/>
       <c r="C125" s="18"/>
       <c r="D125" s="21"/>
@@ -29943,102 +29941,102 @@
     <mergeCell ref="A5:F5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{A3A59D50-FFA7-2949-AAB2-6385AE154B45}"/>
-    <hyperlink ref="G20" r:id="rId2" xr:uid="{6B1F77BD-6439-B448-8655-2DAF8645BCCD}"/>
-    <hyperlink ref="G21" r:id="rId3" xr:uid="{1EA6A34A-7FFE-174A-91A0-EFA0FC09EE93}"/>
-    <hyperlink ref="G22" r:id="rId4" xr:uid="{BA46B661-C624-B84A-8EE4-B1E31ADE62C5}"/>
-    <hyperlink ref="G23" r:id="rId5" xr:uid="{830C5D9C-0166-3143-A560-5B55578001E8}"/>
-    <hyperlink ref="G24" r:id="rId6" xr:uid="{E7480D0B-494E-914E-AB2C-95405B8E8944}"/>
-    <hyperlink ref="G25" r:id="rId7" xr:uid="{950D7355-3836-FB43-B28E-CE86B1C5B81B}"/>
-    <hyperlink ref="G26" r:id="rId8" xr:uid="{D361206A-51D4-FA4A-B48F-27F180164C59}"/>
-    <hyperlink ref="G27" r:id="rId9" xr:uid="{124A95C5-263B-964A-AB56-507E04182013}"/>
-    <hyperlink ref="G28" r:id="rId10" xr:uid="{5D33AF08-9399-6A4B-BE29-2357239D7567}"/>
-    <hyperlink ref="G29" r:id="rId11" xr:uid="{BB1C9B1E-8E3C-B542-8E4D-E45BAA8ABF68}"/>
-    <hyperlink ref="G30" r:id="rId12" xr:uid="{CDCA60C9-0C04-BE46-86D0-D293358D89BB}"/>
-    <hyperlink ref="G31" r:id="rId13" xr:uid="{392312BC-E237-B647-ABBB-BF8472D8CFF2}"/>
-    <hyperlink ref="G32" r:id="rId14" xr:uid="{3357B56C-AB0A-0740-BEF9-0E20B1967C3A}"/>
-    <hyperlink ref="G33" r:id="rId15" xr:uid="{EEEC3045-30AD-8E4E-BA98-EEEF254130B0}"/>
-    <hyperlink ref="G34" r:id="rId16" xr:uid="{B865300C-C180-FE4F-BF43-4EAD3F67DD0A}"/>
-    <hyperlink ref="G35" r:id="rId17" xr:uid="{9EDD187F-B9BF-844C-A8A4-F1D2C7A1CD65}"/>
-    <hyperlink ref="G36" r:id="rId18" xr:uid="{C81DDBE3-E63E-F64D-A415-B6D0CE36E57A}"/>
-    <hyperlink ref="G37" r:id="rId19" xr:uid="{6E765B6F-5012-3043-83F4-57F3F83A65F4}"/>
-    <hyperlink ref="G38" r:id="rId20" xr:uid="{A9E8AE10-391F-1A48-9E24-509D46257907}"/>
-    <hyperlink ref="G39" r:id="rId21" xr:uid="{3ACF6B97-AE0A-8142-BB11-F47F3D53E120}"/>
-    <hyperlink ref="G40" r:id="rId22" xr:uid="{CC794734-127D-3B47-B899-B0F92ADA222F}"/>
-    <hyperlink ref="G41" r:id="rId23" xr:uid="{D9C71EAC-B55B-B04F-B0FF-81696D5302CF}"/>
-    <hyperlink ref="G42" r:id="rId24" xr:uid="{74DC9105-EBBF-5E47-88D7-118DB3EC0455}"/>
-    <hyperlink ref="G43" r:id="rId25" xr:uid="{45C63707-654F-6B45-AB6D-28437008C352}"/>
-    <hyperlink ref="G44" r:id="rId26" xr:uid="{B0DC7C10-40CC-2F42-979F-7DABAC2DA546}"/>
-    <hyperlink ref="G45" r:id="rId27" xr:uid="{727ACF6B-D3C2-BF49-8670-898D62B22EAB}"/>
-    <hyperlink ref="G46" r:id="rId28" xr:uid="{3BA56D63-88F8-324B-B86F-722E3DA5DB0A}"/>
-    <hyperlink ref="G47" r:id="rId29" xr:uid="{624D1919-B1CD-9F42-B6B2-B18A76554559}"/>
-    <hyperlink ref="G48" r:id="rId30" xr:uid="{51FA6C2D-DBF8-4442-BE4E-C3B16377AD75}"/>
-    <hyperlink ref="G49" r:id="rId31" xr:uid="{B1080B3A-8260-D14D-A645-1D49E58590FA}"/>
-    <hyperlink ref="G50" r:id="rId32" xr:uid="{CF6E42CF-B29A-5046-91E6-C3AC1AE24782}"/>
-    <hyperlink ref="G51" r:id="rId33" xr:uid="{F8EE901C-587D-9B44-9A8B-F380A3FCF9E7}"/>
-    <hyperlink ref="G52" r:id="rId34" xr:uid="{40FF4664-4FB3-174F-9F72-718418795B57}"/>
-    <hyperlink ref="G53" r:id="rId35" xr:uid="{66E6744C-059A-FB4D-A1F4-DEB5F51B9E7A}"/>
-    <hyperlink ref="G54" r:id="rId36" xr:uid="{5BF3B7CC-6E6D-8C43-B1C8-A26CC7E9BF93}"/>
-    <hyperlink ref="G55" r:id="rId37" xr:uid="{ACE6E5F0-DA56-DF44-B17D-F889A0087F5F}"/>
-    <hyperlink ref="G56" r:id="rId38" xr:uid="{2D3BD931-EF59-6C45-9E39-8708B643506A}"/>
-    <hyperlink ref="G57" r:id="rId39" xr:uid="{AB266BE8-0C2C-B245-A6CC-E0737FAAF0F9}"/>
-    <hyperlink ref="G58" r:id="rId40" xr:uid="{6E08F784-656F-AD42-82EA-B70635F4CF4D}"/>
-    <hyperlink ref="G59" r:id="rId41" xr:uid="{FCBF69D2-7EC5-1245-A356-4C38FE8922E7}"/>
-    <hyperlink ref="G60" r:id="rId42" xr:uid="{9326ED2B-1E0D-894F-AC7A-3C7EBE9F0028}"/>
-    <hyperlink ref="G61" r:id="rId43" xr:uid="{24854208-92D6-6F4C-9B38-0D6840DF1E11}"/>
-    <hyperlink ref="G62" r:id="rId44" xr:uid="{30E976DE-7B1D-724A-9B00-065A864BD4B5}"/>
-    <hyperlink ref="G63" r:id="rId45" xr:uid="{68731031-DACC-2B4A-861E-7EBA626BD0D2}"/>
-    <hyperlink ref="G64" r:id="rId46" xr:uid="{179684E3-5AB8-5747-B2F2-87263245C3FB}"/>
-    <hyperlink ref="G65" r:id="rId47" xr:uid="{B91C1F7E-D4AA-4946-84DD-D55778203A66}"/>
-    <hyperlink ref="G66" r:id="rId48" xr:uid="{23508AD6-8636-3D4D-A74B-C1EEA8A3775E}"/>
-    <hyperlink ref="G67" r:id="rId49" xr:uid="{88440C0C-4D94-634B-AAB1-C52C104605B3}"/>
-    <hyperlink ref="G68" r:id="rId50" xr:uid="{5367EFF3-75D1-004C-AEBE-70CAE73CECC7}"/>
-    <hyperlink ref="G69" r:id="rId51" xr:uid="{ABBD9663-3890-DD4E-8DEF-4D996FA4059B}"/>
-    <hyperlink ref="G70" r:id="rId52" xr:uid="{3935B5E4-FF18-304D-A5DA-A956FB1B8BC6}"/>
-    <hyperlink ref="G71" r:id="rId53" xr:uid="{F76FFADD-1BAA-444F-AEDD-7EA7098EE0D3}"/>
-    <hyperlink ref="G72" r:id="rId54" xr:uid="{8D3AD4A6-781B-0D4C-A025-D8D2F2AD412B}"/>
-    <hyperlink ref="G73" r:id="rId55" xr:uid="{DD1FA228-B32E-F84F-AFD9-ABC966222D7C}"/>
-    <hyperlink ref="G74" r:id="rId56" xr:uid="{992624A0-DDFD-B846-82CA-8076364FC865}"/>
-    <hyperlink ref="G75" r:id="rId57" xr:uid="{3004FBAA-43D4-A24E-9866-12667FF13974}"/>
-    <hyperlink ref="G76" r:id="rId58" xr:uid="{7D64163C-C127-0544-8CFD-5ADA8A5D3BAA}"/>
-    <hyperlink ref="G77" r:id="rId59" xr:uid="{C1749C20-BE43-4442-98A1-6939AD1ACF83}"/>
-    <hyperlink ref="G78" r:id="rId60" xr:uid="{A5B1EB90-ABBD-4D44-B687-30CC8AFB2083}"/>
-    <hyperlink ref="G79" r:id="rId61" xr:uid="{47BF6E4C-77CC-E54E-B374-6B2E4CA7FC1E}"/>
-    <hyperlink ref="G80" r:id="rId62" xr:uid="{930282A2-9C79-8047-AC79-B7382870FD29}"/>
-    <hyperlink ref="G81" r:id="rId63" xr:uid="{A359AD64-5A3A-6342-916A-74F4F391D96E}"/>
-    <hyperlink ref="G82" r:id="rId64" xr:uid="{4967FCCC-399E-E649-9E53-9DEA3F34BA39}"/>
-    <hyperlink ref="G83" r:id="rId65" xr:uid="{B02427A8-2A6D-5F4E-A485-14B48EF5B603}"/>
-    <hyperlink ref="G84" r:id="rId66" xr:uid="{9785D49F-72E1-6D4E-AF73-FAB16581D509}"/>
-    <hyperlink ref="G85" r:id="rId67" xr:uid="{5A52C361-B79F-3445-B3D4-2B9C639C88B1}"/>
-    <hyperlink ref="G86" r:id="rId68" xr:uid="{C84088EF-8719-994F-A3F5-8CC7121E1C19}"/>
-    <hyperlink ref="G87" r:id="rId69" xr:uid="{1795BBC7-088B-1F40-8188-B17783096206}"/>
-    <hyperlink ref="G88" r:id="rId70" xr:uid="{B81ED23B-4D7F-534A-B5AB-9A2E35B3E8BF}"/>
-    <hyperlink ref="G89" r:id="rId71" xr:uid="{84F84833-F18A-B64D-A539-8A1B925854BB}"/>
-    <hyperlink ref="G90" r:id="rId72" xr:uid="{927BC6C3-92CB-174C-BCB1-77B7C568664D}"/>
-    <hyperlink ref="G91" r:id="rId73" xr:uid="{874C1E8E-E476-EE43-9DA9-BA5241169C83}"/>
-    <hyperlink ref="G92" r:id="rId74" xr:uid="{ADEC8BB7-1A79-CE4C-8415-0350C3DB8C26}"/>
-    <hyperlink ref="G93" r:id="rId75" xr:uid="{F863BB1F-65A2-2B4C-BE74-66884B9BB1D3}"/>
-    <hyperlink ref="G94" r:id="rId76" xr:uid="{EF1F3245-EB86-6944-B43C-5C83386C5F23}"/>
-    <hyperlink ref="G95" r:id="rId77" xr:uid="{B92BA33E-C9FC-AC45-95C0-69E053820374}"/>
-    <hyperlink ref="G96" r:id="rId78" xr:uid="{FB8038A8-0678-5F46-B6B8-E17FBD6E2A7B}"/>
-    <hyperlink ref="G97" r:id="rId79" xr:uid="{F23B60F3-1309-6042-B168-56A2273B8F86}"/>
-    <hyperlink ref="G98" r:id="rId80" xr:uid="{FE102A4F-9E95-8F40-97C7-DED836FE779E}"/>
-    <hyperlink ref="G99" r:id="rId81" xr:uid="{5AB7966A-0C2D-AA4B-A528-CB87477A3BAA}"/>
-    <hyperlink ref="G100" r:id="rId82" xr:uid="{60ED7481-5117-E34B-887C-28DD6F8C6701}"/>
-    <hyperlink ref="G101" r:id="rId83" xr:uid="{C651052A-B73D-1148-B02B-6F81EBC59C4B}"/>
-    <hyperlink ref="G102" r:id="rId84" xr:uid="{F7585C13-E0EA-8043-8C4D-E176500F0454}"/>
-    <hyperlink ref="G103" r:id="rId85" xr:uid="{6B1A0F06-C6A0-E240-B319-04CB3C052B5F}"/>
-    <hyperlink ref="G104" r:id="rId86" xr:uid="{E8CFEC38-62B7-3646-ABD1-CD1B2C063C93}"/>
-    <hyperlink ref="G105" r:id="rId87" xr:uid="{3A3BA951-5CA9-8044-AD9F-6E5DFB39D576}"/>
-    <hyperlink ref="G106" r:id="rId88" xr:uid="{5EFE972E-D99D-1942-A143-AE23BAAE2C2E}"/>
-    <hyperlink ref="G107" r:id="rId89" xr:uid="{3C738773-49CD-BC46-BBD4-A82C731CD595}"/>
-    <hyperlink ref="G108" r:id="rId90" xr:uid="{D2C963B5-889C-0143-A09C-5B3DF3613906}"/>
-    <hyperlink ref="G109" r:id="rId91" xr:uid="{55DC7123-6182-AF41-A30F-5DD1EDF97B60}"/>
-    <hyperlink ref="G110" r:id="rId92" xr:uid="{D431AC73-3DE2-A440-A346-BAAA632B6F3A}"/>
-    <hyperlink ref="G111" r:id="rId93" xr:uid="{EEAD70F5-BBE6-6B4C-B4D9-DD36D742A356}"/>
-    <hyperlink ref="G112" r:id="rId94" xr:uid="{62F62DFA-28B1-7A4D-9B78-6B0CA0D1EB21}"/>
-    <hyperlink ref="G113" r:id="rId95" xr:uid="{1056FB42-B605-0943-A9C6-56B63994AB5D}"/>
-    <hyperlink ref="G114" r:id="rId96" xr:uid="{CD1002D0-ECEC-9941-9954-70B9ED3E37B6}"/>
+    <hyperlink ref="G19" r:id="rId1" display="https://freegenes.github.io/genbank/BBF10K_003373.gb" xr:uid="{A3A59D50-FFA7-2949-AAB2-6385AE154B45}"/>
+    <hyperlink ref="G20" r:id="rId2" display="https://freegenes.github.io/genbank/BBF10K_003375.gb" xr:uid="{6B1F77BD-6439-B448-8655-2DAF8645BCCD}"/>
+    <hyperlink ref="G21" r:id="rId3" display="https://freegenes.github.io/genbank/BBF10K_003376.gb" xr:uid="{1EA6A34A-7FFE-174A-91A0-EFA0FC09EE93}"/>
+    <hyperlink ref="G22" r:id="rId4" display="https://freegenes.github.io/genbank/BBF10K_003378.gb" xr:uid="{BA46B661-C624-B84A-8EE4-B1E31ADE62C5}"/>
+    <hyperlink ref="G23" r:id="rId5" display="https://freegenes.github.io/genbank/BBF10K_003379.gb" xr:uid="{830C5D9C-0166-3143-A560-5B55578001E8}"/>
+    <hyperlink ref="G24" r:id="rId6" display="https://freegenes.github.io/genbank/BBF10K_003380.gb" xr:uid="{E7480D0B-494E-914E-AB2C-95405B8E8944}"/>
+    <hyperlink ref="G25" r:id="rId7" display="https://freegenes.github.io/genbank/BBF10K_003384.gb" xr:uid="{950D7355-3836-FB43-B28E-CE86B1C5B81B}"/>
+    <hyperlink ref="G26" r:id="rId8" display="https://freegenes.github.io/genbank/BBF10K_003385.gb" xr:uid="{D361206A-51D4-FA4A-B48F-27F180164C59}"/>
+    <hyperlink ref="G27" r:id="rId9" display="https://freegenes.github.io/genbank/BBF10K_003386.gb" xr:uid="{124A95C5-263B-964A-AB56-507E04182013}"/>
+    <hyperlink ref="G28" r:id="rId10" display="https://freegenes.github.io/genbank/BBF10K_003387.gb" xr:uid="{5D33AF08-9399-6A4B-BE29-2357239D7567}"/>
+    <hyperlink ref="G29" r:id="rId11" display="https://freegenes.github.io/genbank/BBF10K_003388.gb" xr:uid="{BB1C9B1E-8E3C-B542-8E4D-E45BAA8ABF68}"/>
+    <hyperlink ref="G30" r:id="rId12" display="https://freegenes.github.io/genbank/BBF10K_003389.gb" xr:uid="{CDCA60C9-0C04-BE46-86D0-D293358D89BB}"/>
+    <hyperlink ref="G31" r:id="rId13" display="https://freegenes.github.io/genbank/BBF10K_003390.gb" xr:uid="{392312BC-E237-B647-ABBB-BF8472D8CFF2}"/>
+    <hyperlink ref="G32" r:id="rId14" display="https://freegenes.github.io/genbank/BBF10K_003391.gb" xr:uid="{3357B56C-AB0A-0740-BEF9-0E20B1967C3A}"/>
+    <hyperlink ref="G33" r:id="rId15" display="https://freegenes.github.io/genbank/BBF10K_003392.gb" xr:uid="{EEEC3045-30AD-8E4E-BA98-EEEF254130B0}"/>
+    <hyperlink ref="G34" r:id="rId16" display="https://freegenes.github.io/genbank/BBF10K_003393.gb" xr:uid="{B865300C-C180-FE4F-BF43-4EAD3F67DD0A}"/>
+    <hyperlink ref="G35" r:id="rId17" display="https://freegenes.github.io/genbank/BBF10K_003395.gb" xr:uid="{9EDD187F-B9BF-844C-A8A4-F1D2C7A1CD65}"/>
+    <hyperlink ref="G36" r:id="rId18" display="https://freegenes.github.io/genbank/BBF10K_003396.gb" xr:uid="{C81DDBE3-E63E-F64D-A415-B6D0CE36E57A}"/>
+    <hyperlink ref="G37" r:id="rId19" display="https://freegenes.github.io/genbank/BBF10K_003397.gb" xr:uid="{6E765B6F-5012-3043-83F4-57F3F83A65F4}"/>
+    <hyperlink ref="G38" r:id="rId20" display="https://freegenes.github.io/genbank/BBF10K_003398.gb" xr:uid="{A9E8AE10-391F-1A48-9E24-509D46257907}"/>
+    <hyperlink ref="G39" r:id="rId21" display="https://freegenes.github.io/genbank/BBF10K_003399.gb" xr:uid="{3ACF6B97-AE0A-8142-BB11-F47F3D53E120}"/>
+    <hyperlink ref="G40" r:id="rId22" display="https://freegenes.github.io/genbank/BBF10K_003400.gb" xr:uid="{CC794734-127D-3B47-B899-B0F92ADA222F}"/>
+    <hyperlink ref="G41" r:id="rId23" display="https://freegenes.github.io/genbank/BBF10K_003401.gb" xr:uid="{D9C71EAC-B55B-B04F-B0FF-81696D5302CF}"/>
+    <hyperlink ref="G42" r:id="rId24" display="https://freegenes.github.io/genbank/BBF10K_003402.gb" xr:uid="{74DC9105-EBBF-5E47-88D7-118DB3EC0455}"/>
+    <hyperlink ref="G43" r:id="rId25" display="https://freegenes.github.io/genbank/BBF10K_003403.gb" xr:uid="{45C63707-654F-6B45-AB6D-28437008C352}"/>
+    <hyperlink ref="G44" r:id="rId26" display="https://freegenes.github.io/genbank/BBF10K_003404.gb" xr:uid="{B0DC7C10-40CC-2F42-979F-7DABAC2DA546}"/>
+    <hyperlink ref="G45" r:id="rId27" display="https://freegenes.github.io/genbank/BBF10K_003405.gb" xr:uid="{727ACF6B-D3C2-BF49-8670-898D62B22EAB}"/>
+    <hyperlink ref="G46" r:id="rId28" display="https://freegenes.github.io/genbank/BBF10K_003406.gb" xr:uid="{3BA56D63-88F8-324B-B86F-722E3DA5DB0A}"/>
+    <hyperlink ref="G47" r:id="rId29" display="https://freegenes.github.io/genbank/BBF10K_003407.gb" xr:uid="{624D1919-B1CD-9F42-B6B2-B18A76554559}"/>
+    <hyperlink ref="G48" r:id="rId30" display="https://freegenes.github.io/genbank/BBF10K_003408.gb" xr:uid="{51FA6C2D-DBF8-4442-BE4E-C3B16377AD75}"/>
+    <hyperlink ref="G49" r:id="rId31" display="https://freegenes.github.io/genbank/BBF10K_003409.gb" xr:uid="{B1080B3A-8260-D14D-A645-1D49E58590FA}"/>
+    <hyperlink ref="G50" r:id="rId32" display="https://freegenes.github.io/genbank/BBF10K_003410.gb" xr:uid="{CF6E42CF-B29A-5046-91E6-C3AC1AE24782}"/>
+    <hyperlink ref="G51" r:id="rId33" display="https://freegenes.github.io/genbank/BBF10K_003411.gb" xr:uid="{F8EE901C-587D-9B44-9A8B-F380A3FCF9E7}"/>
+    <hyperlink ref="G52" r:id="rId34" display="https://freegenes.github.io/genbank/BBF10K_003412.gb" xr:uid="{40FF4664-4FB3-174F-9F72-718418795B57}"/>
+    <hyperlink ref="G53" r:id="rId35" display="https://freegenes.github.io/genbank/BBF10K_003413.gb" xr:uid="{66E6744C-059A-FB4D-A1F4-DEB5F51B9E7A}"/>
+    <hyperlink ref="G54" r:id="rId36" display="https://freegenes.github.io/genbank/BBF10K_003414.gb" xr:uid="{5BF3B7CC-6E6D-8C43-B1C8-A26CC7E9BF93}"/>
+    <hyperlink ref="G55" r:id="rId37" display="https://freegenes.github.io/genbank/BBF10K_003415.gb" xr:uid="{ACE6E5F0-DA56-DF44-B17D-F889A0087F5F}"/>
+    <hyperlink ref="G56" r:id="rId38" display="https://freegenes.github.io/genbank/BBF10K_003416.gb" xr:uid="{2D3BD931-EF59-6C45-9E39-8708B643506A}"/>
+    <hyperlink ref="G57" r:id="rId39" display="https://freegenes.github.io/genbank/BBF10K_003417.gb" xr:uid="{AB266BE8-0C2C-B245-A6CC-E0737FAAF0F9}"/>
+    <hyperlink ref="G58" r:id="rId40" display="https://freegenes.github.io/genbank/BBF10K_003418.gb" xr:uid="{6E08F784-656F-AD42-82EA-B70635F4CF4D}"/>
+    <hyperlink ref="G59" r:id="rId41" display="https://freegenes.github.io/genbank/BBF10K_003419.gb" xr:uid="{FCBF69D2-7EC5-1245-A356-4C38FE8922E7}"/>
+    <hyperlink ref="G60" r:id="rId42" display="https://freegenes.github.io/genbank/BBF10K_003420.gb" xr:uid="{9326ED2B-1E0D-894F-AC7A-3C7EBE9F0028}"/>
+    <hyperlink ref="G61" r:id="rId43" display="https://freegenes.github.io/genbank/BBF10K_003421.gb" xr:uid="{24854208-92D6-6F4C-9B38-0D6840DF1E11}"/>
+    <hyperlink ref="G62" r:id="rId44" display="https://freegenes.github.io/genbank/BBF10K_003422.gb" xr:uid="{30E976DE-7B1D-724A-9B00-065A864BD4B5}"/>
+    <hyperlink ref="G63" r:id="rId45" display="https://freegenes.github.io/genbank/BBF10K_003423.gb" xr:uid="{68731031-DACC-2B4A-861E-7EBA626BD0D2}"/>
+    <hyperlink ref="G64" r:id="rId46" display="https://freegenes.github.io/genbank/BBF10K_003424.gb" xr:uid="{179684E3-5AB8-5747-B2F2-87263245C3FB}"/>
+    <hyperlink ref="G65" r:id="rId47" display="https://freegenes.github.io/genbank/BBF10K_003425.gb" xr:uid="{B91C1F7E-D4AA-4946-84DD-D55778203A66}"/>
+    <hyperlink ref="G66" r:id="rId48" display="https://freegenes.github.io/genbank/BBF10K_003426.gb" xr:uid="{23508AD6-8636-3D4D-A74B-C1EEA8A3775E}"/>
+    <hyperlink ref="G67" r:id="rId49" display="https://freegenes.github.io/genbank/BBF10K_003427.gb" xr:uid="{88440C0C-4D94-634B-AAB1-C52C104605B3}"/>
+    <hyperlink ref="G68" r:id="rId50" display="https://freegenes.github.io/genbank/BBF10K_003428.gb" xr:uid="{5367EFF3-75D1-004C-AEBE-70CAE73CECC7}"/>
+    <hyperlink ref="G69" r:id="rId51" display="https://freegenes.github.io/genbank/BBF10K_003429.gb" xr:uid="{ABBD9663-3890-DD4E-8DEF-4D996FA4059B}"/>
+    <hyperlink ref="G70" r:id="rId52" display="https://freegenes.github.io/genbank/BBF10K_003430.gb" xr:uid="{3935B5E4-FF18-304D-A5DA-A956FB1B8BC6}"/>
+    <hyperlink ref="G71" r:id="rId53" display="https://freegenes.github.io/genbank/BBF10K_003431.gb" xr:uid="{F76FFADD-1BAA-444F-AEDD-7EA7098EE0D3}"/>
+    <hyperlink ref="G72" r:id="rId54" display="https://freegenes.github.io/genbank/BBF10K_003432.gb" xr:uid="{8D3AD4A6-781B-0D4C-A025-D8D2F2AD412B}"/>
+    <hyperlink ref="G73" r:id="rId55" display="https://freegenes.github.io/genbank/BBF10K_003433.gb" xr:uid="{DD1FA228-B32E-F84F-AFD9-ABC966222D7C}"/>
+    <hyperlink ref="G74" r:id="rId56" display="https://freegenes.github.io/genbank/BBF10K_003434.gb" xr:uid="{992624A0-DDFD-B846-82CA-8076364FC865}"/>
+    <hyperlink ref="G75" r:id="rId57" display="https://freegenes.github.io/genbank/BBF10K_003436.gb" xr:uid="{3004FBAA-43D4-A24E-9866-12667FF13974}"/>
+    <hyperlink ref="G76" r:id="rId58" display="https://freegenes.github.io/genbank/BBF10K_003437.gb" xr:uid="{7D64163C-C127-0544-8CFD-5ADA8A5D3BAA}"/>
+    <hyperlink ref="G77" r:id="rId59" display="https://freegenes.github.io/genbank/BBF10K_003438.gb" xr:uid="{C1749C20-BE43-4442-98A1-6939AD1ACF83}"/>
+    <hyperlink ref="G78" r:id="rId60" display="https://freegenes.github.io/genbank/BBF10K_003439.gb" xr:uid="{A5B1EB90-ABBD-4D44-B687-30CC8AFB2083}"/>
+    <hyperlink ref="G79" r:id="rId61" display="https://freegenes.github.io/genbank/BBF10K_003440.gb" xr:uid="{47BF6E4C-77CC-E54E-B374-6B2E4CA7FC1E}"/>
+    <hyperlink ref="G80" r:id="rId62" display="https://freegenes.github.io/genbank/BBF10K_003441.gb" xr:uid="{930282A2-9C79-8047-AC79-B7382870FD29}"/>
+    <hyperlink ref="G81" r:id="rId63" display="https://freegenes.github.io/genbank/BBF10K_003442.gb" xr:uid="{A359AD64-5A3A-6342-916A-74F4F391D96E}"/>
+    <hyperlink ref="G82" r:id="rId64" display="https://freegenes.github.io/genbank/BBF10K_003443.gb" xr:uid="{4967FCCC-399E-E649-9E53-9DEA3F34BA39}"/>
+    <hyperlink ref="G83" r:id="rId65" display="https://freegenes.github.io/genbank/BBF10K_003444.gb" xr:uid="{B02427A8-2A6D-5F4E-A485-14B48EF5B603}"/>
+    <hyperlink ref="G84" r:id="rId66" display="https://freegenes.github.io/genbank/BBF10K_003445.gb" xr:uid="{9785D49F-72E1-6D4E-AF73-FAB16581D509}"/>
+    <hyperlink ref="G85" r:id="rId67" display="https://freegenes.github.io/genbank/BBF10K_003446.gb" xr:uid="{5A52C361-B79F-3445-B3D4-2B9C639C88B1}"/>
+    <hyperlink ref="G86" r:id="rId68" display="https://freegenes.github.io/genbank/BBF10K_003447.gb" xr:uid="{C84088EF-8719-994F-A3F5-8CC7121E1C19}"/>
+    <hyperlink ref="G87" r:id="rId69" display="https://freegenes.github.io/genbank/BBF10K_003448.gb" xr:uid="{1795BBC7-088B-1F40-8188-B17783096206}"/>
+    <hyperlink ref="G88" r:id="rId70" display="https://freegenes.github.io/genbank/BBF10K_003449.gb" xr:uid="{B81ED23B-4D7F-534A-B5AB-9A2E35B3E8BF}"/>
+    <hyperlink ref="G89" r:id="rId71" display="https://freegenes.github.io/genbank/BBF10K_003450.gb" xr:uid="{84F84833-F18A-B64D-A539-8A1B925854BB}"/>
+    <hyperlink ref="G90" r:id="rId72" display="https://freegenes.github.io/genbank/BBF10K_003451.gb" xr:uid="{927BC6C3-92CB-174C-BCB1-77B7C568664D}"/>
+    <hyperlink ref="G91" r:id="rId73" display="https://freegenes.github.io/genbank/BBF10K_003452.gb" xr:uid="{874C1E8E-E476-EE43-9DA9-BA5241169C83}"/>
+    <hyperlink ref="G92" r:id="rId74" display="https://freegenes.github.io/genbank/BBF10K_003453.gb" xr:uid="{ADEC8BB7-1A79-CE4C-8415-0350C3DB8C26}"/>
+    <hyperlink ref="G93" r:id="rId75" display="https://freegenes.github.io/genbank/BBF10K_003454.gb" xr:uid="{F863BB1F-65A2-2B4C-BE74-66884B9BB1D3}"/>
+    <hyperlink ref="G94" r:id="rId76" display="https://freegenes.github.io/genbank/BBF10K_003455.gb" xr:uid="{EF1F3245-EB86-6944-B43C-5C83386C5F23}"/>
+    <hyperlink ref="G95" r:id="rId77" display="https://freegenes.github.io/genbank/BBF10K_003457.gb" xr:uid="{B92BA33E-C9FC-AC45-95C0-69E053820374}"/>
+    <hyperlink ref="G96" r:id="rId78" display="https://freegenes.github.io/genbank/BBF10K_003459.gb" xr:uid="{FB8038A8-0678-5F46-B6B8-E17FBD6E2A7B}"/>
+    <hyperlink ref="G97" r:id="rId79" display="https://freegenes.github.io/genbank/BBF10K_003460.gb" xr:uid="{F23B60F3-1309-6042-B168-56A2273B8F86}"/>
+    <hyperlink ref="G98" r:id="rId80" display="https://freegenes.github.io/genbank/BBF10K_003461.gb" xr:uid="{FE102A4F-9E95-8F40-97C7-DED836FE779E}"/>
+    <hyperlink ref="G99" r:id="rId81" display="https://freegenes.github.io/genbank/BBF10K_003462.gb" xr:uid="{5AB7966A-0C2D-AA4B-A528-CB87477A3BAA}"/>
+    <hyperlink ref="G100" r:id="rId82" display="https://freegenes.github.io/genbank/BBF10K_003463.gb" xr:uid="{60ED7481-5117-E34B-887C-28DD6F8C6701}"/>
+    <hyperlink ref="G101" r:id="rId83" display="https://freegenes.github.io/genbank/BBF10K_003464.gb" xr:uid="{C651052A-B73D-1148-B02B-6F81EBC59C4B}"/>
+    <hyperlink ref="G102" r:id="rId84" display="https://freegenes.github.io/genbank/BBF10K_003465.gb" xr:uid="{F7585C13-E0EA-8043-8C4D-E176500F0454}"/>
+    <hyperlink ref="G103" r:id="rId85" display="https://freegenes.github.io/genbank/BBF10K_003466.gb" xr:uid="{6B1A0F06-C6A0-E240-B319-04CB3C052B5F}"/>
+    <hyperlink ref="G104" r:id="rId86" display="https://freegenes.github.io/genbank/BBF10K_003467.gb" xr:uid="{E8CFEC38-62B7-3646-ABD1-CD1B2C063C93}"/>
+    <hyperlink ref="G105" r:id="rId87" display="https://freegenes.github.io/genbank/BBF10K_003468.gb" xr:uid="{3A3BA951-5CA9-8044-AD9F-6E5DFB39D576}"/>
+    <hyperlink ref="G106" r:id="rId88" display="https://freegenes.github.io/genbank/BBF10K_003469.gb" xr:uid="{5EFE972E-D99D-1942-A143-AE23BAAE2C2E}"/>
+    <hyperlink ref="G107" r:id="rId89" display="https://freegenes.github.io/genbank/BBF10K_003470.gb" xr:uid="{3C738773-49CD-BC46-BBD4-A82C731CD595}"/>
+    <hyperlink ref="G108" r:id="rId90" display="https://freegenes.github.io/genbank/BBF10K_003471.gb" xr:uid="{D2C963B5-889C-0143-A09C-5B3DF3613906}"/>
+    <hyperlink ref="G109" r:id="rId91" display="https://freegenes.github.io/genbank/BBF10K_003472.gb" xr:uid="{55DC7123-6182-AF41-A30F-5DD1EDF97B60}"/>
+    <hyperlink ref="G110" r:id="rId92" display="https://freegenes.github.io/genbank/BBF10K_003473.gb" xr:uid="{D431AC73-3DE2-A440-A346-BAAA632B6F3A}"/>
+    <hyperlink ref="G111" r:id="rId93" display="https://freegenes.github.io/genbank/BBF10K_003474.gb" xr:uid="{EEAD70F5-BBE6-6B4C-B4D9-DD36D742A356}"/>
+    <hyperlink ref="G112" r:id="rId94" display="https://freegenes.github.io/genbank/BBF10K_003475.gb" xr:uid="{62F62DFA-28B1-7A4D-9B78-6B0CA0D1EB21}"/>
+    <hyperlink ref="G113" r:id="rId95" display="https://freegenes.github.io/genbank/BBF10K_003476.gb" xr:uid="{1056FB42-B605-0943-A9C6-56B63994AB5D}"/>
+    <hyperlink ref="G114" r:id="rId96" display="https://freegenes.github.io/genbank/BBF10K_003477.gb" xr:uid="{CD1002D0-ECEC-9941-9954-70B9ED3E37B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
changed protein expression kit and open reporters to local
</commit_message>
<xml_diff>
--- a/E coli Protein Expression Toolkit/E coli Protein Expression Toolkit.xlsx
+++ b/E coli Protein Expression Toolkit/E coli Protein Expression Toolkit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/E coli Protein Expression Toolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41098154-5D27-DF4C-9682-C9D886F27B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75E7C40-ABEB-CD42-BAEC-2A908FD3B725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34260" yWindow="3460" windowWidth="30960" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24185,8 +24185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -29940,108 +29940,10 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" display="https://freegenes.github.io/genbank/BBF10K_003373.gb" xr:uid="{A3A59D50-FFA7-2949-AAB2-6385AE154B45}"/>
-    <hyperlink ref="G20" r:id="rId2" display="https://freegenes.github.io/genbank/BBF10K_003375.gb" xr:uid="{6B1F77BD-6439-B448-8655-2DAF8645BCCD}"/>
-    <hyperlink ref="G21" r:id="rId3" display="https://freegenes.github.io/genbank/BBF10K_003376.gb" xr:uid="{1EA6A34A-7FFE-174A-91A0-EFA0FC09EE93}"/>
-    <hyperlink ref="G22" r:id="rId4" display="https://freegenes.github.io/genbank/BBF10K_003378.gb" xr:uid="{BA46B661-C624-B84A-8EE4-B1E31ADE62C5}"/>
-    <hyperlink ref="G23" r:id="rId5" display="https://freegenes.github.io/genbank/BBF10K_003379.gb" xr:uid="{830C5D9C-0166-3143-A560-5B55578001E8}"/>
-    <hyperlink ref="G24" r:id="rId6" display="https://freegenes.github.io/genbank/BBF10K_003380.gb" xr:uid="{E7480D0B-494E-914E-AB2C-95405B8E8944}"/>
-    <hyperlink ref="G25" r:id="rId7" display="https://freegenes.github.io/genbank/BBF10K_003384.gb" xr:uid="{950D7355-3836-FB43-B28E-CE86B1C5B81B}"/>
-    <hyperlink ref="G26" r:id="rId8" display="https://freegenes.github.io/genbank/BBF10K_003385.gb" xr:uid="{D361206A-51D4-FA4A-B48F-27F180164C59}"/>
-    <hyperlink ref="G27" r:id="rId9" display="https://freegenes.github.io/genbank/BBF10K_003386.gb" xr:uid="{124A95C5-263B-964A-AB56-507E04182013}"/>
-    <hyperlink ref="G28" r:id="rId10" display="https://freegenes.github.io/genbank/BBF10K_003387.gb" xr:uid="{5D33AF08-9399-6A4B-BE29-2357239D7567}"/>
-    <hyperlink ref="G29" r:id="rId11" display="https://freegenes.github.io/genbank/BBF10K_003388.gb" xr:uid="{BB1C9B1E-8E3C-B542-8E4D-E45BAA8ABF68}"/>
-    <hyperlink ref="G30" r:id="rId12" display="https://freegenes.github.io/genbank/BBF10K_003389.gb" xr:uid="{CDCA60C9-0C04-BE46-86D0-D293358D89BB}"/>
-    <hyperlink ref="G31" r:id="rId13" display="https://freegenes.github.io/genbank/BBF10K_003390.gb" xr:uid="{392312BC-E237-B647-ABBB-BF8472D8CFF2}"/>
-    <hyperlink ref="G32" r:id="rId14" display="https://freegenes.github.io/genbank/BBF10K_003391.gb" xr:uid="{3357B56C-AB0A-0740-BEF9-0E20B1967C3A}"/>
-    <hyperlink ref="G33" r:id="rId15" display="https://freegenes.github.io/genbank/BBF10K_003392.gb" xr:uid="{EEEC3045-30AD-8E4E-BA98-EEEF254130B0}"/>
-    <hyperlink ref="G34" r:id="rId16" display="https://freegenes.github.io/genbank/BBF10K_003393.gb" xr:uid="{B865300C-C180-FE4F-BF43-4EAD3F67DD0A}"/>
-    <hyperlink ref="G35" r:id="rId17" display="https://freegenes.github.io/genbank/BBF10K_003395.gb" xr:uid="{9EDD187F-B9BF-844C-A8A4-F1D2C7A1CD65}"/>
-    <hyperlink ref="G36" r:id="rId18" display="https://freegenes.github.io/genbank/BBF10K_003396.gb" xr:uid="{C81DDBE3-E63E-F64D-A415-B6D0CE36E57A}"/>
-    <hyperlink ref="G37" r:id="rId19" display="https://freegenes.github.io/genbank/BBF10K_003397.gb" xr:uid="{6E765B6F-5012-3043-83F4-57F3F83A65F4}"/>
-    <hyperlink ref="G38" r:id="rId20" display="https://freegenes.github.io/genbank/BBF10K_003398.gb" xr:uid="{A9E8AE10-391F-1A48-9E24-509D46257907}"/>
-    <hyperlink ref="G39" r:id="rId21" display="https://freegenes.github.io/genbank/BBF10K_003399.gb" xr:uid="{3ACF6B97-AE0A-8142-BB11-F47F3D53E120}"/>
-    <hyperlink ref="G40" r:id="rId22" display="https://freegenes.github.io/genbank/BBF10K_003400.gb" xr:uid="{CC794734-127D-3B47-B899-B0F92ADA222F}"/>
-    <hyperlink ref="G41" r:id="rId23" display="https://freegenes.github.io/genbank/BBF10K_003401.gb" xr:uid="{D9C71EAC-B55B-B04F-B0FF-81696D5302CF}"/>
-    <hyperlink ref="G42" r:id="rId24" display="https://freegenes.github.io/genbank/BBF10K_003402.gb" xr:uid="{74DC9105-EBBF-5E47-88D7-118DB3EC0455}"/>
-    <hyperlink ref="G43" r:id="rId25" display="https://freegenes.github.io/genbank/BBF10K_003403.gb" xr:uid="{45C63707-654F-6B45-AB6D-28437008C352}"/>
-    <hyperlink ref="G44" r:id="rId26" display="https://freegenes.github.io/genbank/BBF10K_003404.gb" xr:uid="{B0DC7C10-40CC-2F42-979F-7DABAC2DA546}"/>
-    <hyperlink ref="G45" r:id="rId27" display="https://freegenes.github.io/genbank/BBF10K_003405.gb" xr:uid="{727ACF6B-D3C2-BF49-8670-898D62B22EAB}"/>
-    <hyperlink ref="G46" r:id="rId28" display="https://freegenes.github.io/genbank/BBF10K_003406.gb" xr:uid="{3BA56D63-88F8-324B-B86F-722E3DA5DB0A}"/>
-    <hyperlink ref="G47" r:id="rId29" display="https://freegenes.github.io/genbank/BBF10K_003407.gb" xr:uid="{624D1919-B1CD-9F42-B6B2-B18A76554559}"/>
-    <hyperlink ref="G48" r:id="rId30" display="https://freegenes.github.io/genbank/BBF10K_003408.gb" xr:uid="{51FA6C2D-DBF8-4442-BE4E-C3B16377AD75}"/>
-    <hyperlink ref="G49" r:id="rId31" display="https://freegenes.github.io/genbank/BBF10K_003409.gb" xr:uid="{B1080B3A-8260-D14D-A645-1D49E58590FA}"/>
-    <hyperlink ref="G50" r:id="rId32" display="https://freegenes.github.io/genbank/BBF10K_003410.gb" xr:uid="{CF6E42CF-B29A-5046-91E6-C3AC1AE24782}"/>
-    <hyperlink ref="G51" r:id="rId33" display="https://freegenes.github.io/genbank/BBF10K_003411.gb" xr:uid="{F8EE901C-587D-9B44-9A8B-F380A3FCF9E7}"/>
-    <hyperlink ref="G52" r:id="rId34" display="https://freegenes.github.io/genbank/BBF10K_003412.gb" xr:uid="{40FF4664-4FB3-174F-9F72-718418795B57}"/>
-    <hyperlink ref="G53" r:id="rId35" display="https://freegenes.github.io/genbank/BBF10K_003413.gb" xr:uid="{66E6744C-059A-FB4D-A1F4-DEB5F51B9E7A}"/>
-    <hyperlink ref="G54" r:id="rId36" display="https://freegenes.github.io/genbank/BBF10K_003414.gb" xr:uid="{5BF3B7CC-6E6D-8C43-B1C8-A26CC7E9BF93}"/>
-    <hyperlink ref="G55" r:id="rId37" display="https://freegenes.github.io/genbank/BBF10K_003415.gb" xr:uid="{ACE6E5F0-DA56-DF44-B17D-F889A0087F5F}"/>
-    <hyperlink ref="G56" r:id="rId38" display="https://freegenes.github.io/genbank/BBF10K_003416.gb" xr:uid="{2D3BD931-EF59-6C45-9E39-8708B643506A}"/>
-    <hyperlink ref="G57" r:id="rId39" display="https://freegenes.github.io/genbank/BBF10K_003417.gb" xr:uid="{AB266BE8-0C2C-B245-A6CC-E0737FAAF0F9}"/>
-    <hyperlink ref="G58" r:id="rId40" display="https://freegenes.github.io/genbank/BBF10K_003418.gb" xr:uid="{6E08F784-656F-AD42-82EA-B70635F4CF4D}"/>
-    <hyperlink ref="G59" r:id="rId41" display="https://freegenes.github.io/genbank/BBF10K_003419.gb" xr:uid="{FCBF69D2-7EC5-1245-A356-4C38FE8922E7}"/>
-    <hyperlink ref="G60" r:id="rId42" display="https://freegenes.github.io/genbank/BBF10K_003420.gb" xr:uid="{9326ED2B-1E0D-894F-AC7A-3C7EBE9F0028}"/>
-    <hyperlink ref="G61" r:id="rId43" display="https://freegenes.github.io/genbank/BBF10K_003421.gb" xr:uid="{24854208-92D6-6F4C-9B38-0D6840DF1E11}"/>
-    <hyperlink ref="G62" r:id="rId44" display="https://freegenes.github.io/genbank/BBF10K_003422.gb" xr:uid="{30E976DE-7B1D-724A-9B00-065A864BD4B5}"/>
-    <hyperlink ref="G63" r:id="rId45" display="https://freegenes.github.io/genbank/BBF10K_003423.gb" xr:uid="{68731031-DACC-2B4A-861E-7EBA626BD0D2}"/>
-    <hyperlink ref="G64" r:id="rId46" display="https://freegenes.github.io/genbank/BBF10K_003424.gb" xr:uid="{179684E3-5AB8-5747-B2F2-87263245C3FB}"/>
-    <hyperlink ref="G65" r:id="rId47" display="https://freegenes.github.io/genbank/BBF10K_003425.gb" xr:uid="{B91C1F7E-D4AA-4946-84DD-D55778203A66}"/>
-    <hyperlink ref="G66" r:id="rId48" display="https://freegenes.github.io/genbank/BBF10K_003426.gb" xr:uid="{23508AD6-8636-3D4D-A74B-C1EEA8A3775E}"/>
-    <hyperlink ref="G67" r:id="rId49" display="https://freegenes.github.io/genbank/BBF10K_003427.gb" xr:uid="{88440C0C-4D94-634B-AAB1-C52C104605B3}"/>
-    <hyperlink ref="G68" r:id="rId50" display="https://freegenes.github.io/genbank/BBF10K_003428.gb" xr:uid="{5367EFF3-75D1-004C-AEBE-70CAE73CECC7}"/>
-    <hyperlink ref="G69" r:id="rId51" display="https://freegenes.github.io/genbank/BBF10K_003429.gb" xr:uid="{ABBD9663-3890-DD4E-8DEF-4D996FA4059B}"/>
-    <hyperlink ref="G70" r:id="rId52" display="https://freegenes.github.io/genbank/BBF10K_003430.gb" xr:uid="{3935B5E4-FF18-304D-A5DA-A956FB1B8BC6}"/>
-    <hyperlink ref="G71" r:id="rId53" display="https://freegenes.github.io/genbank/BBF10K_003431.gb" xr:uid="{F76FFADD-1BAA-444F-AEDD-7EA7098EE0D3}"/>
-    <hyperlink ref="G72" r:id="rId54" display="https://freegenes.github.io/genbank/BBF10K_003432.gb" xr:uid="{8D3AD4A6-781B-0D4C-A025-D8D2F2AD412B}"/>
-    <hyperlink ref="G73" r:id="rId55" display="https://freegenes.github.io/genbank/BBF10K_003433.gb" xr:uid="{DD1FA228-B32E-F84F-AFD9-ABC966222D7C}"/>
-    <hyperlink ref="G74" r:id="rId56" display="https://freegenes.github.io/genbank/BBF10K_003434.gb" xr:uid="{992624A0-DDFD-B846-82CA-8076364FC865}"/>
-    <hyperlink ref="G75" r:id="rId57" display="https://freegenes.github.io/genbank/BBF10K_003436.gb" xr:uid="{3004FBAA-43D4-A24E-9866-12667FF13974}"/>
-    <hyperlink ref="G76" r:id="rId58" display="https://freegenes.github.io/genbank/BBF10K_003437.gb" xr:uid="{7D64163C-C127-0544-8CFD-5ADA8A5D3BAA}"/>
-    <hyperlink ref="G77" r:id="rId59" display="https://freegenes.github.io/genbank/BBF10K_003438.gb" xr:uid="{C1749C20-BE43-4442-98A1-6939AD1ACF83}"/>
-    <hyperlink ref="G78" r:id="rId60" display="https://freegenes.github.io/genbank/BBF10K_003439.gb" xr:uid="{A5B1EB90-ABBD-4D44-B687-30CC8AFB2083}"/>
-    <hyperlink ref="G79" r:id="rId61" display="https://freegenes.github.io/genbank/BBF10K_003440.gb" xr:uid="{47BF6E4C-77CC-E54E-B374-6B2E4CA7FC1E}"/>
-    <hyperlink ref="G80" r:id="rId62" display="https://freegenes.github.io/genbank/BBF10K_003441.gb" xr:uid="{930282A2-9C79-8047-AC79-B7382870FD29}"/>
-    <hyperlink ref="G81" r:id="rId63" display="https://freegenes.github.io/genbank/BBF10K_003442.gb" xr:uid="{A359AD64-5A3A-6342-916A-74F4F391D96E}"/>
-    <hyperlink ref="G82" r:id="rId64" display="https://freegenes.github.io/genbank/BBF10K_003443.gb" xr:uid="{4967FCCC-399E-E649-9E53-9DEA3F34BA39}"/>
-    <hyperlink ref="G83" r:id="rId65" display="https://freegenes.github.io/genbank/BBF10K_003444.gb" xr:uid="{B02427A8-2A6D-5F4E-A485-14B48EF5B603}"/>
-    <hyperlink ref="G84" r:id="rId66" display="https://freegenes.github.io/genbank/BBF10K_003445.gb" xr:uid="{9785D49F-72E1-6D4E-AF73-FAB16581D509}"/>
-    <hyperlink ref="G85" r:id="rId67" display="https://freegenes.github.io/genbank/BBF10K_003446.gb" xr:uid="{5A52C361-B79F-3445-B3D4-2B9C639C88B1}"/>
-    <hyperlink ref="G86" r:id="rId68" display="https://freegenes.github.io/genbank/BBF10K_003447.gb" xr:uid="{C84088EF-8719-994F-A3F5-8CC7121E1C19}"/>
-    <hyperlink ref="G87" r:id="rId69" display="https://freegenes.github.io/genbank/BBF10K_003448.gb" xr:uid="{1795BBC7-088B-1F40-8188-B17783096206}"/>
-    <hyperlink ref="G88" r:id="rId70" display="https://freegenes.github.io/genbank/BBF10K_003449.gb" xr:uid="{B81ED23B-4D7F-534A-B5AB-9A2E35B3E8BF}"/>
-    <hyperlink ref="G89" r:id="rId71" display="https://freegenes.github.io/genbank/BBF10K_003450.gb" xr:uid="{84F84833-F18A-B64D-A539-8A1B925854BB}"/>
-    <hyperlink ref="G90" r:id="rId72" display="https://freegenes.github.io/genbank/BBF10K_003451.gb" xr:uid="{927BC6C3-92CB-174C-BCB1-77B7C568664D}"/>
-    <hyperlink ref="G91" r:id="rId73" display="https://freegenes.github.io/genbank/BBF10K_003452.gb" xr:uid="{874C1E8E-E476-EE43-9DA9-BA5241169C83}"/>
-    <hyperlink ref="G92" r:id="rId74" display="https://freegenes.github.io/genbank/BBF10K_003453.gb" xr:uid="{ADEC8BB7-1A79-CE4C-8415-0350C3DB8C26}"/>
-    <hyperlink ref="G93" r:id="rId75" display="https://freegenes.github.io/genbank/BBF10K_003454.gb" xr:uid="{F863BB1F-65A2-2B4C-BE74-66884B9BB1D3}"/>
-    <hyperlink ref="G94" r:id="rId76" display="https://freegenes.github.io/genbank/BBF10K_003455.gb" xr:uid="{EF1F3245-EB86-6944-B43C-5C83386C5F23}"/>
-    <hyperlink ref="G95" r:id="rId77" display="https://freegenes.github.io/genbank/BBF10K_003457.gb" xr:uid="{B92BA33E-C9FC-AC45-95C0-69E053820374}"/>
-    <hyperlink ref="G96" r:id="rId78" display="https://freegenes.github.io/genbank/BBF10K_003459.gb" xr:uid="{FB8038A8-0678-5F46-B6B8-E17FBD6E2A7B}"/>
-    <hyperlink ref="G97" r:id="rId79" display="https://freegenes.github.io/genbank/BBF10K_003460.gb" xr:uid="{F23B60F3-1309-6042-B168-56A2273B8F86}"/>
-    <hyperlink ref="G98" r:id="rId80" display="https://freegenes.github.io/genbank/BBF10K_003461.gb" xr:uid="{FE102A4F-9E95-8F40-97C7-DED836FE779E}"/>
-    <hyperlink ref="G99" r:id="rId81" display="https://freegenes.github.io/genbank/BBF10K_003462.gb" xr:uid="{5AB7966A-0C2D-AA4B-A528-CB87477A3BAA}"/>
-    <hyperlink ref="G100" r:id="rId82" display="https://freegenes.github.io/genbank/BBF10K_003463.gb" xr:uid="{60ED7481-5117-E34B-887C-28DD6F8C6701}"/>
-    <hyperlink ref="G101" r:id="rId83" display="https://freegenes.github.io/genbank/BBF10K_003464.gb" xr:uid="{C651052A-B73D-1148-B02B-6F81EBC59C4B}"/>
-    <hyperlink ref="G102" r:id="rId84" display="https://freegenes.github.io/genbank/BBF10K_003465.gb" xr:uid="{F7585C13-E0EA-8043-8C4D-E176500F0454}"/>
-    <hyperlink ref="G103" r:id="rId85" display="https://freegenes.github.io/genbank/BBF10K_003466.gb" xr:uid="{6B1A0F06-C6A0-E240-B319-04CB3C052B5F}"/>
-    <hyperlink ref="G104" r:id="rId86" display="https://freegenes.github.io/genbank/BBF10K_003467.gb" xr:uid="{E8CFEC38-62B7-3646-ABD1-CD1B2C063C93}"/>
-    <hyperlink ref="G105" r:id="rId87" display="https://freegenes.github.io/genbank/BBF10K_003468.gb" xr:uid="{3A3BA951-5CA9-8044-AD9F-6E5DFB39D576}"/>
-    <hyperlink ref="G106" r:id="rId88" display="https://freegenes.github.io/genbank/BBF10K_003469.gb" xr:uid="{5EFE972E-D99D-1942-A143-AE23BAAE2C2E}"/>
-    <hyperlink ref="G107" r:id="rId89" display="https://freegenes.github.io/genbank/BBF10K_003470.gb" xr:uid="{3C738773-49CD-BC46-BBD4-A82C731CD595}"/>
-    <hyperlink ref="G108" r:id="rId90" display="https://freegenes.github.io/genbank/BBF10K_003471.gb" xr:uid="{D2C963B5-889C-0143-A09C-5B3DF3613906}"/>
-    <hyperlink ref="G109" r:id="rId91" display="https://freegenes.github.io/genbank/BBF10K_003472.gb" xr:uid="{55DC7123-6182-AF41-A30F-5DD1EDF97B60}"/>
-    <hyperlink ref="G110" r:id="rId92" display="https://freegenes.github.io/genbank/BBF10K_003473.gb" xr:uid="{D431AC73-3DE2-A440-A346-BAAA632B6F3A}"/>
-    <hyperlink ref="G111" r:id="rId93" display="https://freegenes.github.io/genbank/BBF10K_003474.gb" xr:uid="{EEAD70F5-BBE6-6B4C-B4D9-DD36D742A356}"/>
-    <hyperlink ref="G112" r:id="rId94" display="https://freegenes.github.io/genbank/BBF10K_003475.gb" xr:uid="{62F62DFA-28B1-7A4D-9B78-6B0CA0D1EB21}"/>
-    <hyperlink ref="G113" r:id="rId95" display="https://freegenes.github.io/genbank/BBF10K_003476.gb" xr:uid="{1056FB42-B605-0943-A9C6-56B63994AB5D}"/>
-    <hyperlink ref="G114" r:id="rId96" display="https://freegenes.github.io/genbank/BBF10K_003477.gb" xr:uid="{CD1002D0-ECEC-9941-9954-70B9ED3E37B6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId97"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>